<commit_message>
Modified 1 graph in all_data
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctran\OneDrive\Desktop\Coding\csce435project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB82898-62B8-4165-BF26-3BBFF0A19A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C973E2-B394-4416-BEED-897060E577A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,18 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="16">
   <si>
     <t>Processes</t>
   </si>
   <si>
     <t>Input Size</t>
-  </si>
-  <si>
-    <t>Data Ingestion Min</t>
-  </si>
-  <si>
-    <t>Data Ingestion Max</t>
   </si>
   <si>
     <t>Data Ingestion Avg</t>
@@ -70,9 +64,6 @@
   </si>
   <si>
     <t>Sorted Input - Total Gathering Time</t>
-  </si>
-  <si>
-    <t>Data Ingestion Time (Min, Max, Avg)</t>
   </si>
   <si>
     <t>Random Input - Individual Computation Avg</t>
@@ -7889,7 +7880,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Data Ingestion Time vs. # of Processes</a:t>
+              <a:t>Data Ingestion Avg vs. # of Processes</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -7931,10 +7922,86 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="1"/>
+          <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Min (2,560)</c:v>
+            <c:v>2,560</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>256</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Compiled Data'!$C$102:$C$107</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.1700000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.84E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.5300000000000004E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.2700000000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9830000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.8789999999999997E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-EF8B-423B-99FD-54BB7C356DBF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>25,600</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -7975,42 +8042,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compiled Data'!$C$102:$C$107</c:f>
+              <c:f>'Compiled Data'!$C$110:$C$115</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1.0900000000000001E-4</c:v>
+                  <c:v>1.843E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.22E-4</c:v>
+                  <c:v>9.4700000000000003E-4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.31E-4</c:v>
+                  <c:v>9.8900000000000008E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.03E-4</c:v>
+                  <c:v>8.12E-4</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2999999999999999E-5</c:v>
+                  <c:v>5.0270000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.8999999999999997E-5</c:v>
+                  <c:v>6.6990000000000001E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D879-4772-A4BE-01560719908B}"/>
+              <c16:uniqueId val="{00000002-EF8B-423B-99FD-54BB7C356DBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>Max (2,560)</c:v>
+            <c:v>256,000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -8051,42 +8118,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compiled Data'!$D$102:$D$107</c:f>
+              <c:f>'Compiled Data'!$C$118:$C$123</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>4.6799999999999999E-4</c:v>
+                  <c:v>9.8900000000000008E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0269999999999999E-3</c:v>
+                  <c:v>1.2600000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.062E-3</c:v>
+                  <c:v>9.810000000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.859999999999999E-4</c:v>
+                  <c:v>1.1310000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.7995000000000001E-2</c:v>
+                  <c:v>3.8670000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.6887999999999997E-2</c:v>
+                  <c:v>8.1399999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-D879-4772-A4BE-01560719908B}"/>
+              <c16:uniqueId val="{00000003-EF8B-423B-99FD-54BB7C356DBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>Avg (2,560)</c:v>
+            <c:v>2,560,000</c:v>
           </c:tx>
           <c:spPr>
             <a:solidFill>
@@ -8127,730 +8194,34 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Compiled Data'!$E$102:$E$107</c:f>
+              <c:f>'Compiled Data'!$C$126:$C$131</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>3.1700000000000001E-4</c:v>
+                  <c:v>5.4000000000000003E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.84E-4</c:v>
+                  <c:v>2.3600000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.5300000000000004E-4</c:v>
+                  <c:v>1.9369999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2700000000000002E-4</c:v>
+                  <c:v>1.2600000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.9830000000000004E-3</c:v>
+                  <c:v>4.2230000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.8789999999999997E-3</c:v>
+                  <c:v>7.0289999999999997E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:v>Min (25,600)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$C$110:$C$115</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.9900000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.3900000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.0100000000000002E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.6200000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>6.9999999999999994E-5</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.8999999999999997E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="4"/>
-          <c:order val="4"/>
-          <c:tx>
-            <c:v>Max (25,600)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$D$110:$D$115</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.888E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.98E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.5039999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.3489999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0563E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4.3668999999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000006-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:v>Avg (25,600)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$E$110:$E$115</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.843E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>9.4700000000000003E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.8900000000000008E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.12E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.0270000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.6990000000000001E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000007-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="6"/>
-          <c:order val="6"/>
-          <c:tx>
-            <c:v>Min (256,000)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$C$118:$C$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.1000000000000004E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.2800000000000004E-4</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.66E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0899999999999998E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2.5000000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>6.9999999999999994E-5</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000008-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="7"/>
-          <c:order val="7"/>
-          <c:tx>
-            <c:v>Max (256,000)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$D$118:$D$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>1.665E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.709E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.691E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2.0641E-2</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.6920000000000001E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.8998999999999999E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000009-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="11"/>
-          <c:order val="8"/>
-          <c:tx>
-            <c:v>Avg (256,000)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$E$118:$E$123</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>9.8900000000000008E-4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.2600000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.810000000000001E-4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.1310000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.8670000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>8.1399999999999997E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000D-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="8"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:v>Min (2,560,000)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$C$126:$C$131</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3.0959999999999998E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.7279999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.255E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.62E-4</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.27E-4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.7500000000000001E-4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000A-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="10"/>
-          <c:tx>
-            <c:v>Max (2,560,000)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent4">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$D$126:$D$131</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8.0260000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.9510000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.8319999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.823E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1.7656999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.1937E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000B-D879-4772-A4BE-01560719908B}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="10"/>
-          <c:order val="11"/>
-          <c:tx>
-            <c:v>Avg (2,560,000)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent5">
-                <a:lumMod val="60000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Compiled Data'!$A$102:$A$107</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>128</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>256</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Compiled Data'!$E$126:$E$131</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>5.4000000000000003E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.3600000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.9369999999999999E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.2600000000000001E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.2230000000000002E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>7.0289999999999997E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{0000000C-D879-4772-A4BE-01560719908B}"/>
+              <c16:uniqueId val="{00000004-EF8B-423B-99FD-54BB7C356DBF}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -18086,8 +17457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7B859C-9CEF-4DEA-AF23-94F3B0B7BC2A}">
   <dimension ref="A1:X197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F129" sqref="F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18105,12 +17476,12 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="S1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="T1" s="1"/>
       <c r="U1" s="1"/>
@@ -18123,16 +17494,16 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
       </c>
       <c r="S2" t="s">
         <v>0</v>
@@ -18141,16 +17512,16 @@
         <v>1</v>
       </c>
       <c r="U2" t="s">
+        <v>3</v>
+      </c>
+      <c r="V2" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" t="s">
         <v>5</v>
       </c>
-      <c r="V2" t="s">
+      <c r="X2" t="s">
         <v>6</v>
-      </c>
-      <c r="W2" t="s">
-        <v>7</v>
-      </c>
-      <c r="X2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -18281,16 +17652,16 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
+      <c r="F10" t="s">
         <v>6</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
       </c>
       <c r="S10" t="s">
         <v>0</v>
@@ -18299,16 +17670,16 @@
         <v>1</v>
       </c>
       <c r="U10" t="s">
+        <v>3</v>
+      </c>
+      <c r="V10" t="s">
+        <v>4</v>
+      </c>
+      <c r="W10" t="s">
         <v>5</v>
       </c>
-      <c r="V10" t="s">
+      <c r="X10" t="s">
         <v>6</v>
-      </c>
-      <c r="W10" t="s">
-        <v>7</v>
-      </c>
-      <c r="X10" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -18439,16 +17810,16 @@
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>3</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="D18" t="s">
+      <c r="F18" t="s">
         <v>6</v>
-      </c>
-      <c r="E18" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" t="s">
-        <v>8</v>
       </c>
       <c r="S18" t="s">
         <v>0</v>
@@ -18457,16 +17828,16 @@
         <v>1</v>
       </c>
       <c r="U18" t="s">
+        <v>3</v>
+      </c>
+      <c r="V18" t="s">
+        <v>4</v>
+      </c>
+      <c r="W18" t="s">
         <v>5</v>
       </c>
-      <c r="V18" t="s">
+      <c r="X18" t="s">
         <v>6</v>
-      </c>
-      <c r="W18" t="s">
-        <v>7</v>
-      </c>
-      <c r="X18" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
@@ -18597,16 +17968,16 @@
         <v>1</v>
       </c>
       <c r="C26" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" t="s">
+        <v>4</v>
+      </c>
+      <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="D26" t="s">
+      <c r="F26" t="s">
         <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>8</v>
       </c>
       <c r="S26" t="s">
         <v>0</v>
@@ -18615,16 +17986,16 @@
         <v>1</v>
       </c>
       <c r="U26" t="s">
+        <v>3</v>
+      </c>
+      <c r="V26" t="s">
+        <v>4</v>
+      </c>
+      <c r="W26" t="s">
         <v>5</v>
       </c>
-      <c r="V26" t="s">
+      <c r="X26" t="s">
         <v>6</v>
-      </c>
-      <c r="W26" t="s">
-        <v>7</v>
-      </c>
-      <c r="X26" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
@@ -18749,12 +18120,12 @@
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="S34" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
@@ -18767,16 +18138,16 @@
         <v>1</v>
       </c>
       <c r="C35" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" t="s">
         <v>5</v>
       </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
         <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-      <c r="F35" t="s">
-        <v>8</v>
       </c>
       <c r="S35" t="s">
         <v>0</v>
@@ -18785,16 +18156,16 @@
         <v>1</v>
       </c>
       <c r="U35" t="s">
+        <v>3</v>
+      </c>
+      <c r="V35" t="s">
+        <v>4</v>
+      </c>
+      <c r="W35" t="s">
         <v>5</v>
       </c>
-      <c r="V35" t="s">
+      <c r="X35" t="s">
         <v>6</v>
-      </c>
-      <c r="W35" t="s">
-        <v>7</v>
-      </c>
-      <c r="X35" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.25">
@@ -18925,16 +18296,16 @@
         <v>1</v>
       </c>
       <c r="C43" t="s">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
+        <v>4</v>
+      </c>
+      <c r="E43" t="s">
         <v>5</v>
       </c>
-      <c r="D43" t="s">
+      <c r="F43" t="s">
         <v>6</v>
-      </c>
-      <c r="E43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>8</v>
       </c>
       <c r="S43" t="s">
         <v>0</v>
@@ -18943,16 +18314,16 @@
         <v>1</v>
       </c>
       <c r="U43" t="s">
+        <v>3</v>
+      </c>
+      <c r="V43" t="s">
+        <v>4</v>
+      </c>
+      <c r="W43" t="s">
         <v>5</v>
       </c>
-      <c r="V43" t="s">
+      <c r="X43" t="s">
         <v>6</v>
-      </c>
-      <c r="W43" t="s">
-        <v>7</v>
-      </c>
-      <c r="X43" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="44" spans="1:24" x14ac:dyDescent="0.25">
@@ -19083,16 +18454,16 @@
         <v>1</v>
       </c>
       <c r="C51" t="s">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" t="s">
         <v>5</v>
       </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
         <v>6</v>
-      </c>
-      <c r="E51" t="s">
-        <v>7</v>
-      </c>
-      <c r="F51" t="s">
-        <v>8</v>
       </c>
       <c r="S51" t="s">
         <v>0</v>
@@ -19101,16 +18472,16 @@
         <v>1</v>
       </c>
       <c r="U51" t="s">
+        <v>3</v>
+      </c>
+      <c r="V51" t="s">
+        <v>4</v>
+      </c>
+      <c r="W51" t="s">
         <v>5</v>
       </c>
-      <c r="V51" t="s">
+      <c r="X51" t="s">
         <v>6</v>
-      </c>
-      <c r="W51" t="s">
-        <v>7</v>
-      </c>
-      <c r="X51" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.25">
@@ -19241,16 +18612,16 @@
         <v>1</v>
       </c>
       <c r="C59" t="s">
+        <v>3</v>
+      </c>
+      <c r="D59" t="s">
+        <v>4</v>
+      </c>
+      <c r="E59" t="s">
         <v>5</v>
       </c>
-      <c r="D59" t="s">
+      <c r="F59" t="s">
         <v>6</v>
-      </c>
-      <c r="E59" t="s">
-        <v>7</v>
-      </c>
-      <c r="F59" t="s">
-        <v>8</v>
       </c>
       <c r="S59" t="s">
         <v>0</v>
@@ -19259,16 +18630,16 @@
         <v>1</v>
       </c>
       <c r="U59" t="s">
+        <v>3</v>
+      </c>
+      <c r="V59" t="s">
+        <v>4</v>
+      </c>
+      <c r="W59" t="s">
         <v>5</v>
       </c>
-      <c r="V59" t="s">
+      <c r="X59" t="s">
         <v>6</v>
-      </c>
-      <c r="W59" t="s">
-        <v>7</v>
-      </c>
-      <c r="X59" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
@@ -19393,12 +18764,12 @@
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="S67" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="T67" s="1"/>
       <c r="U67" s="1"/>
@@ -19411,16 +18782,16 @@
         <v>1</v>
       </c>
       <c r="C68" t="s">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
+        <v>4</v>
+      </c>
+      <c r="E68" t="s">
         <v>5</v>
       </c>
-      <c r="D68" t="s">
+      <c r="F68" t="s">
         <v>6</v>
-      </c>
-      <c r="E68" t="s">
-        <v>7</v>
-      </c>
-      <c r="F68" t="s">
-        <v>8</v>
       </c>
       <c r="S68" t="s">
         <v>0</v>
@@ -19429,16 +18800,16 @@
         <v>1</v>
       </c>
       <c r="U68" t="s">
+        <v>3</v>
+      </c>
+      <c r="V68" t="s">
+        <v>4</v>
+      </c>
+      <c r="W68" t="s">
         <v>5</v>
       </c>
-      <c r="V68" t="s">
+      <c r="X68" t="s">
         <v>6</v>
-      </c>
-      <c r="W68" t="s">
-        <v>7</v>
-      </c>
-      <c r="X68" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
@@ -19569,16 +18940,16 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
+        <v>4</v>
+      </c>
+      <c r="E76" t="s">
         <v>5</v>
       </c>
-      <c r="D76" t="s">
+      <c r="F76" t="s">
         <v>6</v>
-      </c>
-      <c r="E76" t="s">
-        <v>7</v>
-      </c>
-      <c r="F76" t="s">
-        <v>8</v>
       </c>
       <c r="S76" t="s">
         <v>0</v>
@@ -19587,16 +18958,16 @@
         <v>1</v>
       </c>
       <c r="U76" t="s">
+        <v>3</v>
+      </c>
+      <c r="V76" t="s">
+        <v>4</v>
+      </c>
+      <c r="W76" t="s">
         <v>5</v>
       </c>
-      <c r="V76" t="s">
+      <c r="X76" t="s">
         <v>6</v>
-      </c>
-      <c r="W76" t="s">
-        <v>7</v>
-      </c>
-      <c r="X76" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="77" spans="1:24" x14ac:dyDescent="0.25">
@@ -19727,16 +19098,16 @@
         <v>1</v>
       </c>
       <c r="C84" t="s">
+        <v>3</v>
+      </c>
+      <c r="D84" t="s">
+        <v>4</v>
+      </c>
+      <c r="E84" t="s">
         <v>5</v>
       </c>
-      <c r="D84" t="s">
+      <c r="F84" t="s">
         <v>6</v>
-      </c>
-      <c r="E84" t="s">
-        <v>7</v>
-      </c>
-      <c r="F84" t="s">
-        <v>8</v>
       </c>
       <c r="S84" t="s">
         <v>0</v>
@@ -19745,16 +19116,16 @@
         <v>1</v>
       </c>
       <c r="U84" t="s">
+        <v>3</v>
+      </c>
+      <c r="V84" t="s">
+        <v>4</v>
+      </c>
+      <c r="W84" t="s">
         <v>5</v>
       </c>
-      <c r="V84" t="s">
+      <c r="X84" t="s">
         <v>6</v>
-      </c>
-      <c r="W84" t="s">
-        <v>7</v>
-      </c>
-      <c r="X84" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
@@ -19885,16 +19256,16 @@
         <v>1</v>
       </c>
       <c r="C92" t="s">
+        <v>3</v>
+      </c>
+      <c r="D92" t="s">
+        <v>4</v>
+      </c>
+      <c r="E92" t="s">
         <v>5</v>
       </c>
-      <c r="D92" t="s">
+      <c r="F92" t="s">
         <v>6</v>
-      </c>
-      <c r="E92" t="s">
-        <v>7</v>
-      </c>
-      <c r="F92" t="s">
-        <v>8</v>
       </c>
       <c r="S92" t="s">
         <v>0</v>
@@ -19903,16 +19274,16 @@
         <v>1</v>
       </c>
       <c r="U92" t="s">
+        <v>3</v>
+      </c>
+      <c r="V92" t="s">
+        <v>4</v>
+      </c>
+      <c r="W92" t="s">
         <v>5</v>
       </c>
-      <c r="V92" t="s">
+      <c r="X92" t="s">
         <v>6</v>
-      </c>
-      <c r="W92" t="s">
-        <v>7</v>
-      </c>
-      <c r="X92" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="93" spans="1:24" x14ac:dyDescent="0.25">
@@ -20037,12 +19408,12 @@
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="S100" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="T100" s="1"/>
       <c r="U100" s="1"/>
@@ -20057,12 +19428,6 @@
       <c r="C101" t="s">
         <v>2</v>
       </c>
-      <c r="D101" t="s">
-        <v>3</v>
-      </c>
-      <c r="E101" t="s">
-        <v>4</v>
-      </c>
       <c r="S101" t="s">
         <v>0</v>
       </c>
@@ -20070,16 +19435,16 @@
         <v>1</v>
       </c>
       <c r="U101" t="s">
+        <v>3</v>
+      </c>
+      <c r="V101" t="s">
+        <v>4</v>
+      </c>
+      <c r="W101" t="s">
         <v>5</v>
       </c>
-      <c r="V101" t="s">
+      <c r="X101" t="s">
         <v>6</v>
-      </c>
-      <c r="W101" t="s">
-        <v>7</v>
-      </c>
-      <c r="X101" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.25">
@@ -20090,12 +19455,6 @@
         <v>2560</v>
       </c>
       <c r="C102">
-        <v>1.0900000000000001E-4</v>
-      </c>
-      <c r="D102">
-        <v>4.6799999999999999E-4</v>
-      </c>
-      <c r="E102">
         <v>3.1700000000000001E-4</v>
       </c>
       <c r="S102">
@@ -20116,12 +19475,6 @@
         <v>2560</v>
       </c>
       <c r="C103">
-        <v>1.22E-4</v>
-      </c>
-      <c r="D103">
-        <v>1.0269999999999999E-3</v>
-      </c>
-      <c r="E103">
         <v>4.84E-4</v>
       </c>
       <c r="S103">
@@ -20142,12 +19495,6 @@
         <v>2560</v>
       </c>
       <c r="C104">
-        <v>2.31E-4</v>
-      </c>
-      <c r="D104">
-        <v>1.062E-3</v>
-      </c>
-      <c r="E104">
         <v>6.5300000000000004E-4</v>
       </c>
       <c r="S104">
@@ -20168,12 +19515,6 @@
         <v>2560</v>
       </c>
       <c r="C105">
-        <v>1.03E-4</v>
-      </c>
-      <c r="D105">
-        <v>9.859999999999999E-4</v>
-      </c>
-      <c r="E105">
         <v>5.2700000000000002E-4</v>
       </c>
       <c r="S105">
@@ -20194,12 +19535,6 @@
         <v>2560</v>
       </c>
       <c r="C106">
-        <v>7.2999999999999999E-5</v>
-      </c>
-      <c r="D106">
-        <v>1.7995000000000001E-2</v>
-      </c>
-      <c r="E106">
         <v>3.9830000000000004E-3</v>
       </c>
       <c r="S106">
@@ -20220,12 +19555,6 @@
         <v>2560</v>
       </c>
       <c r="C107">
-        <v>6.8999999999999997E-5</v>
-      </c>
-      <c r="D107">
-        <v>3.6887999999999997E-2</v>
-      </c>
-      <c r="E107">
         <v>6.8789999999999997E-3</v>
       </c>
       <c r="S107">
@@ -20248,12 +19577,6 @@
       <c r="C109" t="s">
         <v>2</v>
       </c>
-      <c r="D109" t="s">
-        <v>3</v>
-      </c>
-      <c r="E109" t="s">
-        <v>4</v>
-      </c>
       <c r="S109" t="s">
         <v>0</v>
       </c>
@@ -20261,16 +19584,16 @@
         <v>1</v>
       </c>
       <c r="U109" t="s">
+        <v>3</v>
+      </c>
+      <c r="V109" t="s">
+        <v>4</v>
+      </c>
+      <c r="W109" t="s">
         <v>5</v>
       </c>
-      <c r="V109" t="s">
+      <c r="X109" t="s">
         <v>6</v>
-      </c>
-      <c r="W109" t="s">
-        <v>7</v>
-      </c>
-      <c r="X109" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="110" spans="1:24" x14ac:dyDescent="0.25">
@@ -20281,12 +19604,6 @@
         <v>25600</v>
       </c>
       <c r="C110">
-        <v>5.9900000000000003E-4</v>
-      </c>
-      <c r="D110">
-        <v>5.888E-3</v>
-      </c>
-      <c r="E110">
         <v>1.843E-3</v>
       </c>
       <c r="S110">
@@ -20307,12 +19624,6 @@
         <v>25600</v>
       </c>
       <c r="C111">
-        <v>2.3900000000000001E-4</v>
-      </c>
-      <c r="D111">
-        <v>1.98E-3</v>
-      </c>
-      <c r="E111">
         <v>9.4700000000000003E-4</v>
       </c>
       <c r="S111">
@@ -20333,12 +19644,6 @@
         <v>25600</v>
       </c>
       <c r="C112">
-        <v>7.0100000000000002E-4</v>
-      </c>
-      <c r="D112">
-        <v>1.5039999999999999E-3</v>
-      </c>
-      <c r="E112">
         <v>9.8900000000000008E-4</v>
       </c>
       <c r="S112">
@@ -20359,12 +19664,6 @@
         <v>25600</v>
       </c>
       <c r="C113">
-        <v>1.6200000000000001E-4</v>
-      </c>
-      <c r="D113">
-        <v>1.3489999999999999E-3</v>
-      </c>
-      <c r="E113">
         <v>8.12E-4</v>
       </c>
       <c r="S113">
@@ -20385,12 +19684,6 @@
         <v>25600</v>
       </c>
       <c r="C114">
-        <v>6.9999999999999994E-5</v>
-      </c>
-      <c r="D114">
-        <v>3.0563E-2</v>
-      </c>
-      <c r="E114">
         <v>5.0270000000000002E-3</v>
       </c>
       <c r="S114">
@@ -20411,12 +19704,6 @@
         <v>25600</v>
       </c>
       <c r="C115">
-        <v>6.8999999999999997E-5</v>
-      </c>
-      <c r="D115">
-        <v>4.3668999999999999E-2</v>
-      </c>
-      <c r="E115">
         <v>6.6990000000000001E-3</v>
       </c>
       <c r="S115">
@@ -20439,12 +19726,6 @@
       <c r="C117" t="s">
         <v>2</v>
       </c>
-      <c r="D117" t="s">
-        <v>3</v>
-      </c>
-      <c r="E117" t="s">
-        <v>4</v>
-      </c>
       <c r="S117" t="s">
         <v>0</v>
       </c>
@@ -20452,16 +19733,16 @@
         <v>1</v>
       </c>
       <c r="U117" t="s">
+        <v>3</v>
+      </c>
+      <c r="V117" t="s">
+        <v>4</v>
+      </c>
+      <c r="W117" t="s">
         <v>5</v>
       </c>
-      <c r="V117" t="s">
+      <c r="X117" t="s">
         <v>6</v>
-      </c>
-      <c r="W117" t="s">
-        <v>7</v>
-      </c>
-      <c r="X117" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="118" spans="1:24" x14ac:dyDescent="0.25">
@@ -20472,12 +19753,6 @@
         <v>256000</v>
       </c>
       <c r="C118">
-        <v>5.1000000000000004E-4</v>
-      </c>
-      <c r="D118">
-        <v>1.665E-3</v>
-      </c>
-      <c r="E118">
         <v>9.8900000000000008E-4</v>
       </c>
       <c r="S118">
@@ -20498,12 +19773,6 @@
         <v>256000</v>
       </c>
       <c r="C119">
-        <v>5.2800000000000004E-4</v>
-      </c>
-      <c r="D119">
-        <v>2.709E-3</v>
-      </c>
-      <c r="E119">
         <v>1.2600000000000001E-3</v>
       </c>
       <c r="S119">
@@ -20524,12 +19793,6 @@
         <v>256000</v>
       </c>
       <c r="C120">
-        <v>4.66E-4</v>
-      </c>
-      <c r="D120">
-        <v>1.691E-3</v>
-      </c>
-      <c r="E120">
         <v>9.810000000000001E-4</v>
       </c>
       <c r="S120">
@@ -20550,12 +19813,6 @@
         <v>256000</v>
       </c>
       <c r="C121">
-        <v>3.0899999999999998E-4</v>
-      </c>
-      <c r="D121">
-        <v>2.0641E-2</v>
-      </c>
-      <c r="E121">
         <v>1.1310000000000001E-3</v>
       </c>
       <c r="S121">
@@ -20576,12 +19833,6 @@
         <v>256000</v>
       </c>
       <c r="C122">
-        <v>2.5000000000000001E-4</v>
-      </c>
-      <c r="D122">
-        <v>1.6920000000000001E-2</v>
-      </c>
-      <c r="E122">
         <v>3.8670000000000002E-3</v>
       </c>
       <c r="S122">
@@ -20602,12 +19853,6 @@
         <v>256000</v>
       </c>
       <c r="C123">
-        <v>6.9999999999999994E-5</v>
-      </c>
-      <c r="D123">
-        <v>3.8998999999999999E-2</v>
-      </c>
-      <c r="E123">
         <v>8.1399999999999997E-3</v>
       </c>
       <c r="S123">
@@ -20630,12 +19875,6 @@
       <c r="C125" t="s">
         <v>2</v>
       </c>
-      <c r="D125" t="s">
-        <v>3</v>
-      </c>
-      <c r="E125" t="s">
-        <v>4</v>
-      </c>
       <c r="S125" t="s">
         <v>0</v>
       </c>
@@ -20643,16 +19882,16 @@
         <v>1</v>
       </c>
       <c r="U125" t="s">
+        <v>3</v>
+      </c>
+      <c r="V125" t="s">
+        <v>4</v>
+      </c>
+      <c r="W125" t="s">
         <v>5</v>
       </c>
-      <c r="V125" t="s">
+      <c r="X125" t="s">
         <v>6</v>
-      </c>
-      <c r="W125" t="s">
-        <v>7</v>
-      </c>
-      <c r="X125" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="126" spans="1:24" x14ac:dyDescent="0.25">
@@ -20663,12 +19902,6 @@
         <v>2560000</v>
       </c>
       <c r="C126">
-        <v>3.0959999999999998E-3</v>
-      </c>
-      <c r="D126">
-        <v>8.0260000000000001E-3</v>
-      </c>
-      <c r="E126">
         <v>5.4000000000000003E-3</v>
       </c>
       <c r="S126">
@@ -20689,12 +19922,6 @@
         <v>2560000</v>
       </c>
       <c r="C127">
-        <v>1.7279999999999999E-3</v>
-      </c>
-      <c r="D127">
-        <v>2.9510000000000001E-3</v>
-      </c>
-      <c r="E127">
         <v>2.3600000000000001E-3</v>
       </c>
       <c r="S127">
@@ -20715,12 +19942,6 @@
         <v>2560000</v>
       </c>
       <c r="C128">
-        <v>1.255E-3</v>
-      </c>
-      <c r="D128">
-        <v>2.8319999999999999E-3</v>
-      </c>
-      <c r="E128">
         <v>1.9369999999999999E-3</v>
       </c>
       <c r="S128">
@@ -20741,12 +19962,6 @@
         <v>2560000</v>
       </c>
       <c r="C129">
-        <v>5.62E-4</v>
-      </c>
-      <c r="D129">
-        <v>1.823E-3</v>
-      </c>
-      <c r="E129">
         <v>1.2600000000000001E-3</v>
       </c>
       <c r="S129">
@@ -20767,12 +19982,6 @@
         <v>2560000</v>
       </c>
       <c r="C130">
-        <v>1.27E-4</v>
-      </c>
-      <c r="D130">
-        <v>1.7656999999999999E-2</v>
-      </c>
-      <c r="E130">
         <v>4.2230000000000002E-3</v>
       </c>
       <c r="S130">
@@ -20793,12 +20002,6 @@
         <v>2560000</v>
       </c>
       <c r="C131">
-        <v>3.7500000000000001E-4</v>
-      </c>
-      <c r="D131">
-        <v>3.1937E-2</v>
-      </c>
-      <c r="E131">
         <v>7.0289999999999997E-3</v>
       </c>
       <c r="S131">
@@ -20813,7 +20016,7 @@
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S133" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="T133" s="1"/>
       <c r="U133" s="1"/>
@@ -20826,16 +20029,16 @@
         <v>1</v>
       </c>
       <c r="U134" t="s">
+        <v>3</v>
+      </c>
+      <c r="V134" t="s">
+        <v>4</v>
+      </c>
+      <c r="W134" t="s">
         <v>5</v>
       </c>
-      <c r="V134" t="s">
+      <c r="X134" t="s">
         <v>6</v>
-      </c>
-      <c r="W134" t="s">
-        <v>7</v>
-      </c>
-      <c r="X134" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="135" spans="1:24" x14ac:dyDescent="0.25">
@@ -20912,16 +20115,16 @@
         <v>1</v>
       </c>
       <c r="U142" t="s">
+        <v>3</v>
+      </c>
+      <c r="V142" t="s">
+        <v>4</v>
+      </c>
+      <c r="W142" t="s">
         <v>5</v>
       </c>
-      <c r="V142" t="s">
+      <c r="X142" t="s">
         <v>6</v>
-      </c>
-      <c r="W142" t="s">
-        <v>7</v>
-      </c>
-      <c r="X142" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.25">
@@ -20998,16 +20201,16 @@
         <v>1</v>
       </c>
       <c r="U150" t="s">
+        <v>3</v>
+      </c>
+      <c r="V150" t="s">
+        <v>4</v>
+      </c>
+      <c r="W150" t="s">
         <v>5</v>
       </c>
-      <c r="V150" t="s">
+      <c r="X150" t="s">
         <v>6</v>
-      </c>
-      <c r="W150" t="s">
-        <v>7</v>
-      </c>
-      <c r="X150" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="151" spans="19:24" x14ac:dyDescent="0.25">
@@ -21084,16 +20287,16 @@
         <v>1</v>
       </c>
       <c r="U158" t="s">
+        <v>3</v>
+      </c>
+      <c r="V158" t="s">
+        <v>4</v>
+      </c>
+      <c r="W158" t="s">
         <v>5</v>
       </c>
-      <c r="V158" t="s">
+      <c r="X158" t="s">
         <v>6</v>
-      </c>
-      <c r="W158" t="s">
-        <v>7</v>
-      </c>
-      <c r="X158" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="159" spans="19:24" x14ac:dyDescent="0.25">
@@ -21164,7 +20367,7 @@
     </row>
     <row r="166" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S166" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="T166" s="1"/>
       <c r="U166" s="1"/>
@@ -21177,16 +20380,16 @@
         <v>1</v>
       </c>
       <c r="U167" t="s">
+        <v>3</v>
+      </c>
+      <c r="V167" t="s">
+        <v>4</v>
+      </c>
+      <c r="W167" t="s">
         <v>5</v>
       </c>
-      <c r="V167" t="s">
+      <c r="X167" t="s">
         <v>6</v>
-      </c>
-      <c r="W167" t="s">
-        <v>7</v>
-      </c>
-      <c r="X167" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="168" spans="19:24" x14ac:dyDescent="0.25">
@@ -21263,16 +20466,16 @@
         <v>1</v>
       </c>
       <c r="U175" t="s">
+        <v>3</v>
+      </c>
+      <c r="V175" t="s">
+        <v>4</v>
+      </c>
+      <c r="W175" t="s">
         <v>5</v>
       </c>
-      <c r="V175" t="s">
+      <c r="X175" t="s">
         <v>6</v>
-      </c>
-      <c r="W175" t="s">
-        <v>7</v>
-      </c>
-      <c r="X175" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="176" spans="19:24" x14ac:dyDescent="0.25">
@@ -21349,16 +20552,16 @@
         <v>1</v>
       </c>
       <c r="U183" t="s">
+        <v>3</v>
+      </c>
+      <c r="V183" t="s">
+        <v>4</v>
+      </c>
+      <c r="W183" t="s">
         <v>5</v>
       </c>
-      <c r="V183" t="s">
+      <c r="X183" t="s">
         <v>6</v>
-      </c>
-      <c r="W183" t="s">
-        <v>7</v>
-      </c>
-      <c r="X183" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="184" spans="19:24" x14ac:dyDescent="0.25">
@@ -21435,16 +20638,16 @@
         <v>1</v>
       </c>
       <c r="U191" t="s">
+        <v>3</v>
+      </c>
+      <c r="V191" t="s">
+        <v>4</v>
+      </c>
+      <c r="W191" t="s">
         <v>5</v>
       </c>
-      <c r="V191" t="s">
+      <c r="X191" t="s">
         <v>6</v>
-      </c>
-      <c r="W191" t="s">
-        <v>7</v>
-      </c>
-      <c r="X191" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="192" spans="19:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added ParallelMergeSort data to all_data.xlsx
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctran\OneDrive\Desktop\Coding\csce435project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\siraius\Class_Files\CSCE435\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C973E2-B394-4416-BEED-897060E577A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07F90DC9-3BEB-4816-8A07-508DACE512F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10290" yWindow="4110" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled Data" sheetId="4" r:id="rId1"/>
@@ -411,6 +411,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.8869999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8318000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0058999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6011000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.3562999999999993E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.34959099999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -582,6 +600,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4194E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4081999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2880000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0288999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1009000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.112997</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -732,6 +768,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.1519999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.1215E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0942000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.8743000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9242999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8211000000000007E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -885,6 +939,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.15631900000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.15681400000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.168438</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17200599999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38206499999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.87575800000000004</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1512,6 +1584,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.4000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4999999999999994E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000002E-6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1683,6 +1773,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.7999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5999999999999999E-5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1833,6 +1941,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.3499999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8299999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0000000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4999999999999997E-5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1986,6 +2112,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.2019999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0340000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1510000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3209999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0700000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.1800000000000002E-4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2613,6 +2757,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.7006E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5479999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6084000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4081E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7832000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.105521</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2784,6 +2946,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.4900000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6797999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2382000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.7281999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1410000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23064699999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2934,6 +3114,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.9953000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5596000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8975999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5992999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7111000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16659599999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3087,6 +3285,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.1209999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.0212000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.110887</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.8781999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.198708</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.56554700000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3714,6 +3930,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.7080000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1963E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9942E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5923E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3751E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17565700000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -3885,6 +4119,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.4910000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9172000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0755E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7890000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1765E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16472999999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4035,6 +4287,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.7614E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9433999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6836000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4745999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5581E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16339799999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4188,6 +4458,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>9.9562999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.2874999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.109123</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16328699999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.183536</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46755000000000002</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4815,6 +5103,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>5.4380000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7894E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.9638E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5611999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9904000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.32938699999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4986,6 +5292,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3442000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3601E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2437000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9740999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.8210999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.10834000000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5136,6 +5460,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.7518999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9149000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9187999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.802E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.5854000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8047999999999996E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5289,6 +5631,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.11808100000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.138021</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.159805</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16744700000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.37980599999999998</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.85675699999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5916,6 +6276,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6605999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4756E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.4955E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3153000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9919E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.6848000000000004E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6087,6 +6465,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.6859999999999993E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6269000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0828000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6936E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5180000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23055899999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6237,6 +6633,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.8799E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4545999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.801E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5808999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.6985000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.152951</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6390,6 +6804,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.1754999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4830000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.10824499999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.7577999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.19812199999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55332700000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7017,6 +7449,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6695999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1194000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9525E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5346E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.2127999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.169073</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7188,6 +7638,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.5779999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8615E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0323999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.214E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.9046000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13297500000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7338,6 +7806,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5940000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8344999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5185000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4556000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0690000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.160995</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7491,6 +7977,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.9981000000000005E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8151999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.1856999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.16197600000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.170323</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.46067200000000003</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8804,6 +9308,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.6999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.9999999999999999E-6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.9999999999999996E-6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9056,6 +9578,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.7399999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.36E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.2000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6999999999999997E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.6999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.12E-4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9314,6 +9854,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.3909999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.555E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.1299999999999998E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6099999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8699999999999999E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.7000000000000001E-5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9575,6 +10133,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.6357E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7686E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7899999999999992E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.9379999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.215E-3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3749999999999999E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10229,6 +10805,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.0999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6999999999999999E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.5000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5000000000000006E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0000000000000002E-6</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10481,6 +11075,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.2999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.0000000000000002E-5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5999999999999998E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3999999999999998E-5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10739,6 +11351,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.0799999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8699999999999997E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.92E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.08E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3000000000000001E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.4E-5</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11000,6 +11630,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.3829999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.823E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.853E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0799999999999995E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.1600000000000001E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.4899999999999998E-4</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -17457,8 +18105,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7B859C-9CEF-4DEA-AF23-94F3B0B7BC2A}">
   <dimension ref="A1:X197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="F129" sqref="F129"/>
+    <sheetView tabSelected="1" topLeftCell="Q136" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y153" sqref="Y153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17534,6 +18182,9 @@
       <c r="C3">
         <v>1.8991999999999998E-2</v>
       </c>
+      <c r="E3">
+        <v>5.8869999999999999E-3</v>
+      </c>
       <c r="S3">
         <v>8</v>
       </c>
@@ -17542,6 +18193,9 @@
       </c>
       <c r="U3">
         <v>2.4810000000000001E-3</v>
+      </c>
+      <c r="W3">
+        <v>5.4380000000000001E-3</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -17554,6 +18208,9 @@
       <c r="C4">
         <v>2.2852999999999998E-2</v>
       </c>
+      <c r="E4">
+        <v>1.8318000000000001E-2</v>
+      </c>
       <c r="S4">
         <v>16</v>
       </c>
@@ -17562,6 +18219,9 @@
       </c>
       <c r="U4">
         <v>1.797E-3</v>
+      </c>
+      <c r="W4">
+        <v>1.7894E-2</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -17574,6 +18234,9 @@
       <c r="C5">
         <v>3.1753999999999998E-2</v>
       </c>
+      <c r="E5">
+        <v>4.0058999999999997E-2</v>
+      </c>
       <c r="S5">
         <v>32</v>
       </c>
@@ -17582,6 +18245,9 @@
       </c>
       <c r="U5">
         <v>2.2989999999999998E-3</v>
+      </c>
+      <c r="W5">
+        <v>3.9638E-2</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -17594,6 +18260,9 @@
       <c r="C6">
         <v>5.6314000000000003E-2</v>
       </c>
+      <c r="E6">
+        <v>1.6011000000000001E-2</v>
+      </c>
       <c r="S6">
         <v>64</v>
       </c>
@@ -17602,6 +18271,9 @@
       </c>
       <c r="U6">
         <v>9.9120000000000007E-3</v>
+      </c>
+      <c r="W6">
+        <v>1.5611999999999999E-2</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -17614,6 +18286,9 @@
       <c r="C7">
         <v>2.4154469999999999</v>
       </c>
+      <c r="E7">
+        <v>9.3562999999999993E-2</v>
+      </c>
       <c r="S7">
         <v>128</v>
       </c>
@@ -17622,6 +18297,9 @@
       </c>
       <c r="U7">
         <v>0.57863799999999999</v>
+      </c>
+      <c r="W7">
+        <v>7.9904000000000003E-2</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -17634,6 +18312,9 @@
       <c r="C8">
         <v>6.3815869999999997</v>
       </c>
+      <c r="E8">
+        <v>0.34959099999999999</v>
+      </c>
       <c r="S8">
         <v>256</v>
       </c>
@@ -17642,6 +18323,9 @@
       </c>
       <c r="U8">
         <v>0.75822199999999995</v>
+      </c>
+      <c r="W8">
+        <v>0.32938699999999999</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -17692,6 +18376,9 @@
       <c r="C11">
         <v>2.9548000000000001E-2</v>
       </c>
+      <c r="E11">
+        <v>1.4194E-2</v>
+      </c>
       <c r="S11">
         <v>8</v>
       </c>
@@ -17700,6 +18387,9 @@
       </c>
       <c r="U11">
         <v>8.3429999999999997E-3</v>
+      </c>
+      <c r="W11">
+        <v>1.3442000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -17712,6 +18402,9 @@
       <c r="C12">
         <v>2.1846000000000001E-2</v>
       </c>
+      <c r="E12">
+        <v>2.4081999999999999E-2</v>
+      </c>
       <c r="S12">
         <v>16</v>
       </c>
@@ -17720,6 +18413,9 @@
       </c>
       <c r="U12">
         <v>4.1289999999999999E-3</v>
+      </c>
+      <c r="W12">
+        <v>2.3601E-2</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -17732,6 +18428,9 @@
       <c r="C13">
         <v>2.3531E-2</v>
       </c>
+      <c r="E13">
+        <v>4.2880000000000001E-2</v>
+      </c>
       <c r="S13">
         <v>32</v>
       </c>
@@ -17740,6 +18439,9 @@
       </c>
       <c r="U13">
         <v>4.8209999999999998E-3</v>
+      </c>
+      <c r="W13">
+        <v>4.2437000000000002E-2</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -17752,6 +18454,9 @@
       <c r="C14">
         <v>2.9329000000000001E-2</v>
       </c>
+      <c r="E14">
+        <v>4.0288999999999998E-2</v>
+      </c>
       <c r="S14">
         <v>64</v>
       </c>
@@ -17760,6 +18465,9 @@
       </c>
       <c r="U14">
         <v>1.1608E-2</v>
+      </c>
+      <c r="W14">
+        <v>3.9740999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
@@ -17772,6 +18480,9 @@
       <c r="C15">
         <v>2.2690769999999998</v>
       </c>
+      <c r="E15">
+        <v>7.1009000000000003E-2</v>
+      </c>
       <c r="S15">
         <v>128</v>
       </c>
@@ -17780,6 +18491,9 @@
       </c>
       <c r="U15">
         <v>0.52526200000000001</v>
+      </c>
+      <c r="W15">
+        <v>6.8210999999999994E-2</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
@@ -17792,6 +18506,9 @@
       <c r="C16">
         <v>6.0244169999999997</v>
       </c>
+      <c r="E16">
+        <v>0.112997</v>
+      </c>
       <c r="S16">
         <v>256</v>
       </c>
@@ -17800,6 +18517,9 @@
       </c>
       <c r="U16">
         <v>0.61958800000000003</v>
+      </c>
+      <c r="W16">
+        <v>0.10834000000000001</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
@@ -17850,6 +18570,9 @@
       <c r="C19">
         <v>2.9779E-2</v>
       </c>
+      <c r="E19">
+        <v>3.1519999999999999E-2</v>
+      </c>
       <c r="S19">
         <v>8</v>
       </c>
@@ -17858,6 +18581,9 @@
       </c>
       <c r="U19">
         <v>2.6340000000000001E-3</v>
+      </c>
+      <c r="W19">
+        <v>2.7518999999999998E-2</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -17870,6 +18596,9 @@
       <c r="C20">
         <v>4.0583000000000001E-2</v>
       </c>
+      <c r="E20">
+        <v>3.1215E-2</v>
+      </c>
       <c r="S20">
         <v>16</v>
       </c>
@@ -17878,6 +18607,9 @@
       </c>
       <c r="U20">
         <v>7.7299999999999999E-3</v>
+      </c>
+      <c r="W20">
+        <v>2.9149000000000001E-2</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
@@ -17890,6 +18622,9 @@
       <c r="C21">
         <v>6.3003000000000003E-2</v>
       </c>
+      <c r="E21">
+        <v>6.0942000000000003E-2</v>
+      </c>
       <c r="S21">
         <v>32</v>
       </c>
@@ -17898,6 +18633,9 @@
       </c>
       <c r="U21">
         <v>3.6709999999999998E-3</v>
+      </c>
+      <c r="W21">
+        <v>5.9187999999999998E-2</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -17910,6 +18648,9 @@
       <c r="C22">
         <v>5.0469E-2</v>
       </c>
+      <c r="E22">
+        <v>2.8743000000000001E-2</v>
+      </c>
       <c r="S22">
         <v>64</v>
       </c>
@@ -17918,6 +18659,9 @@
       </c>
       <c r="U22">
         <v>4.3499999999999997E-3</v>
+      </c>
+      <c r="W22">
+        <v>2.802E-2</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
@@ -17930,6 +18674,9 @@
       <c r="C23">
         <v>2.42191</v>
       </c>
+      <c r="E23">
+        <v>7.9242999999999994E-2</v>
+      </c>
       <c r="S23">
         <v>128</v>
       </c>
@@ -17938,6 +18685,9 @@
       </c>
       <c r="U23">
         <v>0.28568100000000002</v>
+      </c>
+      <c r="W23">
+        <v>7.5854000000000005E-2</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
@@ -17950,6 +18700,9 @@
       <c r="C24">
         <v>6.0383659999999999</v>
       </c>
+      <c r="E24">
+        <v>9.8211000000000007E-2</v>
+      </c>
       <c r="S24">
         <v>256</v>
       </c>
@@ -17958,6 +18711,9 @@
       </c>
       <c r="U24">
         <v>0.119743</v>
+      </c>
+      <c r="W24">
+        <v>9.8047999999999996E-2</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
@@ -18008,6 +18764,9 @@
       <c r="C27">
         <v>0.279362</v>
       </c>
+      <c r="E27">
+        <v>0.15631900000000001</v>
+      </c>
       <c r="S27">
         <v>8</v>
       </c>
@@ -18016,6 +18775,9 @@
       </c>
       <c r="U27">
         <v>2.4039999999999999E-2</v>
+      </c>
+      <c r="W27">
+        <v>0.11808100000000001</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
@@ -18028,6 +18790,9 @@
       <c r="C28">
         <v>0.24790100000000001</v>
       </c>
+      <c r="E28">
+        <v>0.15681400000000001</v>
+      </c>
       <c r="S28">
         <v>16</v>
       </c>
@@ -18036,6 +18801,9 @@
       </c>
       <c r="U28">
         <v>2.1049999999999999E-2</v>
+      </c>
+      <c r="W28">
+        <v>0.138021</v>
       </c>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
@@ -18048,6 +18816,9 @@
       <c r="C29">
         <v>0.27188299999999999</v>
       </c>
+      <c r="E29">
+        <v>0.168438</v>
+      </c>
       <c r="S29">
         <v>32</v>
       </c>
@@ -18056,6 +18827,9 @@
       </c>
       <c r="U29">
         <v>6.868E-3</v>
+      </c>
+      <c r="W29">
+        <v>0.159805</v>
       </c>
     </row>
     <row r="30" spans="1:24" x14ac:dyDescent="0.25">
@@ -18068,6 +18842,9 @@
       <c r="C30">
         <v>0.19980600000000001</v>
       </c>
+      <c r="E30">
+        <v>0.17200599999999999</v>
+      </c>
       <c r="S30">
         <v>64</v>
       </c>
@@ -18076,6 +18853,9 @@
       </c>
       <c r="U30">
         <v>1.0076E-2</v>
+      </c>
+      <c r="W30">
+        <v>0.16744700000000001</v>
       </c>
     </row>
     <row r="31" spans="1:24" x14ac:dyDescent="0.25">
@@ -18088,6 +18868,9 @@
       <c r="C31">
         <v>2.011768</v>
       </c>
+      <c r="E31">
+        <v>0.38206499999999999</v>
+      </c>
       <c r="S31">
         <v>128</v>
       </c>
@@ -18096,6 +18879,9 @@
       </c>
       <c r="U31">
         <v>0.107583</v>
+      </c>
+      <c r="W31">
+        <v>0.37980599999999998</v>
       </c>
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
@@ -18108,6 +18894,9 @@
       <c r="C32">
         <v>7.6345970000000003</v>
       </c>
+      <c r="E32">
+        <v>0.87575800000000004</v>
+      </c>
       <c r="S32">
         <v>256</v>
       </c>
@@ -18116,6 +18905,9 @@
       </c>
       <c r="U32">
         <v>1.970982</v>
+      </c>
+      <c r="W32">
+        <v>0.85675699999999999</v>
       </c>
     </row>
     <row r="34" spans="1:24" x14ac:dyDescent="0.25">
@@ -18178,6 +18970,9 @@
       <c r="C36">
         <v>1.8464000000000001E-2</v>
       </c>
+      <c r="E36">
+        <v>1.7006E-2</v>
+      </c>
       <c r="S36">
         <v>8</v>
       </c>
@@ -18186,6 +18981,9 @@
       </c>
       <c r="U36">
         <v>1.441E-3</v>
+      </c>
+      <c r="W36">
+        <v>1.6605999999999999E-2</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.25">
@@ -18198,6 +18996,9 @@
       <c r="C37">
         <v>2.1499000000000001E-2</v>
       </c>
+      <c r="E37">
+        <v>2.5479999999999999E-2</v>
+      </c>
       <c r="S37">
         <v>16</v>
       </c>
@@ -18206,6 +19007,9 @@
       </c>
       <c r="U37">
         <v>1.21E-4</v>
+      </c>
+      <c r="W37">
+        <v>2.4756E-2</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.25">
@@ -18218,6 +19022,9 @@
       <c r="C38">
         <v>3.6063999999999999E-2</v>
       </c>
+      <c r="E38">
+        <v>1.6084000000000001E-2</v>
+      </c>
       <c r="S38">
         <v>32</v>
       </c>
@@ -18226,6 +19033,9 @@
       </c>
       <c r="U38">
         <v>2.415E-3</v>
+      </c>
+      <c r="W38">
+        <v>1.4955E-2</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.25">
@@ -18238,6 +19048,9 @@
       <c r="C39">
         <v>2.7976000000000001E-2</v>
       </c>
+      <c r="E39">
+        <v>3.4081E-2</v>
+      </c>
       <c r="S39">
         <v>64</v>
       </c>
@@ -18246,6 +19059,9 @@
       </c>
       <c r="U39">
         <v>5.0540000000000003E-3</v>
+      </c>
+      <c r="W39">
+        <v>3.3153000000000002E-2</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.25">
@@ -18258,6 +19074,9 @@
       <c r="C40">
         <v>2.3998430000000002</v>
       </c>
+      <c r="E40">
+        <v>6.7832000000000003E-2</v>
+      </c>
       <c r="S40">
         <v>128</v>
       </c>
@@ -18266,6 +19085,9 @@
       </c>
       <c r="U40">
         <v>0.39906399999999997</v>
+      </c>
+      <c r="W40">
+        <v>5.9919E-2</v>
       </c>
     </row>
     <row r="41" spans="1:24" x14ac:dyDescent="0.25">
@@ -18278,6 +19100,9 @@
       <c r="C41">
         <v>7.2779059999999998</v>
       </c>
+      <c r="E41">
+        <v>0.105521</v>
+      </c>
       <c r="S41">
         <v>256</v>
       </c>
@@ -18286,6 +19111,9 @@
       </c>
       <c r="U41">
         <v>1.0944199999999999</v>
+      </c>
+      <c r="W41">
+        <v>9.6848000000000004E-2</v>
       </c>
     </row>
     <row r="43" spans="1:24" x14ac:dyDescent="0.25">
@@ -18336,6 +19164,9 @@
       <c r="C44">
         <v>4.1079999999999998E-2</v>
       </c>
+      <c r="E44">
+        <v>9.4900000000000002E-3</v>
+      </c>
       <c r="S44">
         <v>8</v>
       </c>
@@ -18344,6 +19175,9 @@
       </c>
       <c r="U44">
         <v>1.418E-3</v>
+      </c>
+      <c r="W44">
+        <v>8.6859999999999993E-3</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
@@ -18356,6 +19190,9 @@
       <c r="C45">
         <v>2.9602E-2</v>
       </c>
+      <c r="E45">
+        <v>2.6797999999999999E-2</v>
+      </c>
       <c r="S45">
         <v>16</v>
       </c>
@@ -18364,6 +19201,9 @@
       </c>
       <c r="U45">
         <v>1.06E-3</v>
+      </c>
+      <c r="W45">
+        <v>2.6269000000000001E-2</v>
       </c>
     </row>
     <row r="46" spans="1:24" x14ac:dyDescent="0.25">
@@ -18376,6 +19216,9 @@
       <c r="C46">
         <v>4.2826000000000003E-2</v>
       </c>
+      <c r="E46">
+        <v>3.2382000000000001E-2</v>
+      </c>
       <c r="S46">
         <v>32</v>
       </c>
@@ -18384,6 +19227,9 @@
       </c>
       <c r="U46">
         <v>2.745E-3</v>
+      </c>
+      <c r="W46">
+        <v>3.0828000000000001E-2</v>
       </c>
     </row>
     <row r="47" spans="1:24" x14ac:dyDescent="0.25">
@@ -18396,6 +19242,9 @@
       <c r="C47">
         <v>3.6757999999999999E-2</v>
       </c>
+      <c r="E47">
+        <v>1.7281999999999999E-2</v>
+      </c>
       <c r="S47">
         <v>64</v>
       </c>
@@ -18404,6 +19253,9 @@
       </c>
       <c r="U47">
         <v>1.7856E-2</v>
+      </c>
+      <c r="W47">
+        <v>1.6936E-2</v>
       </c>
     </row>
     <row r="48" spans="1:24" x14ac:dyDescent="0.25">
@@ -18416,6 +19268,9 @@
       <c r="C48">
         <v>2.54297</v>
       </c>
+      <c r="E48">
+        <v>7.1410000000000001E-2</v>
+      </c>
       <c r="S48">
         <v>128</v>
       </c>
@@ -18424,6 +19279,9 @@
       </c>
       <c r="U48">
         <v>0.31934299999999999</v>
+      </c>
+      <c r="W48">
+        <v>6.5180000000000002E-2</v>
       </c>
     </row>
     <row r="49" spans="1:24" x14ac:dyDescent="0.25">
@@ -18436,6 +19294,9 @@
       <c r="C49">
         <v>6.1158130000000002</v>
       </c>
+      <c r="E49">
+        <v>0.23064699999999999</v>
+      </c>
       <c r="S49">
         <v>256</v>
       </c>
@@ -18444,6 +19305,9 @@
       </c>
       <c r="U49">
         <v>0.97077100000000005</v>
+      </c>
+      <c r="W49">
+        <v>0.23055899999999999</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.25">
@@ -18494,6 +19358,9 @@
       <c r="C52">
         <v>3.4171E-2</v>
       </c>
+      <c r="E52">
+        <v>3.9953000000000002E-2</v>
+      </c>
       <c r="S52">
         <v>8</v>
       </c>
@@ -18502,6 +19369,9 @@
       </c>
       <c r="U52">
         <v>4.5259999999999996E-3</v>
+      </c>
+      <c r="W52">
+        <v>3.8799E-2</v>
       </c>
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.25">
@@ -18514,6 +19384,9 @@
       <c r="C53">
         <v>3.7383E-2</v>
       </c>
+      <c r="E53">
+        <v>2.5596000000000001E-2</v>
+      </c>
       <c r="S53">
         <v>16</v>
       </c>
@@ -18522,6 +19395,9 @@
       </c>
       <c r="U53">
         <v>3.6480000000000002E-3</v>
+      </c>
+      <c r="W53">
+        <v>2.4545999999999998E-2</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.25">
@@ -18534,6 +19410,9 @@
       <c r="C54">
         <v>5.5820000000000002E-2</v>
       </c>
+      <c r="E54">
+        <v>2.8975999999999998E-2</v>
+      </c>
       <c r="S54">
         <v>32</v>
       </c>
@@ -18542,6 +19421,9 @@
       </c>
       <c r="U54">
         <v>2.1020000000000001E-3</v>
+      </c>
+      <c r="W54">
+        <v>2.801E-2</v>
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
@@ -18554,6 +19436,9 @@
       <c r="C55">
         <v>3.7256999999999998E-2</v>
       </c>
+      <c r="E55">
+        <v>2.5992999999999999E-2</v>
+      </c>
       <c r="S55">
         <v>64</v>
       </c>
@@ -18562,6 +19447,9 @@
       </c>
       <c r="U55">
         <v>4.1479999999999998E-3</v>
+      </c>
+      <c r="W55">
+        <v>2.5808999999999999E-2</v>
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
@@ -18574,6 +19462,9 @@
       <c r="C56">
         <v>2.51715</v>
       </c>
+      <c r="E56">
+        <v>6.7111000000000004E-2</v>
+      </c>
       <c r="S56">
         <v>128</v>
       </c>
@@ -18582,6 +19473,9 @@
       </c>
       <c r="U56">
         <v>0.686608</v>
+      </c>
+      <c r="W56">
+        <v>6.6985000000000003E-2</v>
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
@@ -18594,6 +19488,9 @@
       <c r="C57">
         <v>6.9820229999999999</v>
       </c>
+      <c r="E57">
+        <v>0.16659599999999999</v>
+      </c>
       <c r="S57">
         <v>256</v>
       </c>
@@ -18602,6 +19499,9 @@
       </c>
       <c r="U57">
         <v>0.62252700000000005</v>
+      </c>
+      <c r="W57">
+        <v>0.152951</v>
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
@@ -18652,6 +19552,9 @@
       <c r="C60">
         <v>0.208455</v>
       </c>
+      <c r="E60">
+        <v>9.1209999999999999E-2</v>
+      </c>
       <c r="S60">
         <v>8</v>
       </c>
@@ -18660,6 +19563,9 @@
       </c>
       <c r="U60">
         <v>2.5004999999999999E-2</v>
+      </c>
+      <c r="W60">
+        <v>8.1754999999999994E-2</v>
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
@@ -18672,6 +19578,9 @@
       <c r="C61">
         <v>0.20402200000000001</v>
       </c>
+      <c r="E61">
+        <v>9.0212000000000001E-2</v>
+      </c>
       <c r="S61">
         <v>16</v>
       </c>
@@ -18680,6 +19589,9 @@
       </c>
       <c r="U61">
         <v>1.4725E-2</v>
+      </c>
+      <c r="W61">
+        <v>8.4830000000000003E-2</v>
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
@@ -18692,6 +19604,9 @@
       <c r="C62">
         <v>0.305008</v>
       </c>
+      <c r="E62">
+        <v>0.110887</v>
+      </c>
       <c r="S62">
         <v>32</v>
       </c>
@@ -18700,6 +19615,9 @@
       </c>
       <c r="U62">
         <v>8.9840000000000007E-3</v>
+      </c>
+      <c r="W62">
+        <v>0.10824499999999999</v>
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
@@ -18712,6 +19630,9 @@
       <c r="C63">
         <v>0.214027</v>
       </c>
+      <c r="E63">
+        <v>9.8781999999999995E-2</v>
+      </c>
       <c r="S63">
         <v>64</v>
       </c>
@@ -18720,6 +19641,9 @@
       </c>
       <c r="U63">
         <v>9.4859999999999996E-3</v>
+      </c>
+      <c r="W63">
+        <v>9.7577999999999998E-2</v>
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
@@ -18732,6 +19656,9 @@
       <c r="C64">
         <v>2.4375369999999998</v>
       </c>
+      <c r="E64">
+        <v>0.198708</v>
+      </c>
       <c r="S64">
         <v>128</v>
       </c>
@@ -18740,6 +19667,9 @@
       </c>
       <c r="U64">
         <v>0.41578100000000001</v>
+      </c>
+      <c r="W64">
+        <v>0.19812199999999999</v>
       </c>
     </row>
     <row r="65" spans="1:24" x14ac:dyDescent="0.25">
@@ -18752,6 +19682,9 @@
       <c r="C65">
         <v>7.7045240000000002</v>
       </c>
+      <c r="E65">
+        <v>0.56554700000000002</v>
+      </c>
       <c r="S65">
         <v>256</v>
       </c>
@@ -18760,6 +19693,9 @@
       </c>
       <c r="U65">
         <v>1.0215540000000001</v>
+      </c>
+      <c r="W65">
+        <v>0.55332700000000001</v>
       </c>
     </row>
     <row r="67" spans="1:24" x14ac:dyDescent="0.25">
@@ -18822,6 +19758,9 @@
       <c r="C69">
         <v>1.3576E-2</v>
       </c>
+      <c r="E69">
+        <v>1.7080000000000001E-2</v>
+      </c>
       <c r="S69">
         <v>8</v>
       </c>
@@ -18830,6 +19769,9 @@
       </c>
       <c r="U69">
         <v>2.3289999999999999E-3</v>
+      </c>
+      <c r="W69">
+        <v>1.6695999999999999E-2</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
@@ -18842,6 +19784,9 @@
       <c r="C70">
         <v>3.5298999999999997E-2</v>
       </c>
+      <c r="E70">
+        <v>1.1963E-2</v>
+      </c>
       <c r="S70">
         <v>16</v>
       </c>
@@ -18850,6 +19795,9 @@
       </c>
       <c r="U70">
         <v>1.743E-3</v>
+      </c>
+      <c r="W70">
+        <v>1.1194000000000001E-2</v>
       </c>
     </row>
     <row r="71" spans="1:24" x14ac:dyDescent="0.25">
@@ -18862,6 +19810,9 @@
       <c r="C71">
         <v>3.6466999999999999E-2</v>
       </c>
+      <c r="E71">
+        <v>4.9942E-2</v>
+      </c>
       <c r="S71">
         <v>32</v>
       </c>
@@ -18870,6 +19821,9 @@
       </c>
       <c r="U71">
         <v>9.0989999999999994E-3</v>
+      </c>
+      <c r="W71">
+        <v>4.9525E-2</v>
       </c>
     </row>
     <row r="72" spans="1:24" x14ac:dyDescent="0.25">
@@ -18882,6 +19836,9 @@
       <c r="C72">
         <v>2.1936000000000001E-2</v>
       </c>
+      <c r="E72">
+        <v>1.5923E-2</v>
+      </c>
       <c r="S72">
         <v>64</v>
       </c>
@@ -18890,6 +19847,9 @@
       </c>
       <c r="U72">
         <v>8.8850000000000005E-3</v>
+      </c>
+      <c r="W72">
+        <v>1.5346E-2</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
@@ -18902,6 +19862,9 @@
       <c r="C73">
         <v>2.533982</v>
       </c>
+      <c r="E73">
+        <v>5.3751E-2</v>
+      </c>
       <c r="S73">
         <v>128</v>
       </c>
@@ -18910,6 +19873,9 @@
       </c>
       <c r="U73">
         <v>0.279339</v>
+      </c>
+      <c r="W73">
+        <v>4.2127999999999999E-2</v>
       </c>
     </row>
     <row r="74" spans="1:24" x14ac:dyDescent="0.25">
@@ -18922,6 +19888,9 @@
       <c r="C74">
         <v>7.3390789999999999</v>
       </c>
+      <c r="E74">
+        <v>0.17565700000000001</v>
+      </c>
       <c r="S74">
         <v>256</v>
       </c>
@@ -18930,6 +19899,9 @@
       </c>
       <c r="U74">
         <v>1.467549</v>
+      </c>
+      <c r="W74">
+        <v>0.169073</v>
       </c>
     </row>
     <row r="76" spans="1:24" x14ac:dyDescent="0.25">
@@ -18980,6 +19952,9 @@
       <c r="C77">
         <v>1.6687E-2</v>
       </c>
+      <c r="E77">
+        <v>8.4910000000000003E-3</v>
+      </c>
       <c r="S77">
         <v>8</v>
       </c>
@@ -18988,6 +19963,9 @@
       </c>
       <c r="U77">
         <v>2.6800000000000001E-4</v>
+      </c>
+      <c r="W77">
+        <v>7.5779999999999997E-3</v>
       </c>
     </row>
     <row r="78" spans="1:24" x14ac:dyDescent="0.25">
@@ -19000,6 +19978,9 @@
       <c r="C78">
         <v>2.2144E-2</v>
       </c>
+      <c r="E78">
+        <v>1.9172000000000002E-2</v>
+      </c>
       <c r="S78">
         <v>16</v>
       </c>
@@ -19008,6 +19989,9 @@
       </c>
       <c r="U78">
         <v>4.653E-3</v>
+      </c>
+      <c r="W78">
+        <v>1.8615E-2</v>
       </c>
     </row>
     <row r="79" spans="1:24" x14ac:dyDescent="0.25">
@@ -19020,6 +20004,9 @@
       <c r="C79">
         <v>4.0250000000000001E-2</v>
       </c>
+      <c r="E79">
+        <v>4.0755E-2</v>
+      </c>
       <c r="S79">
         <v>32</v>
       </c>
@@ -19028,6 +20015,9 @@
       </c>
       <c r="U79">
         <v>1.76E-4</v>
+      </c>
+      <c r="W79">
+        <v>4.0323999999999999E-2</v>
       </c>
     </row>
     <row r="80" spans="1:24" x14ac:dyDescent="0.25">
@@ -19040,6 +20030,9 @@
       <c r="C80">
         <v>5.2542999999999999E-2</v>
       </c>
+      <c r="E80">
+        <v>9.7890000000000008E-3</v>
+      </c>
       <c r="S80">
         <v>64</v>
       </c>
@@ -19048,6 +20041,9 @@
       </c>
       <c r="U80">
         <v>4.4939999999999997E-3</v>
+      </c>
+      <c r="W80">
+        <v>9.214E-3</v>
       </c>
     </row>
     <row r="81" spans="1:24" x14ac:dyDescent="0.25">
@@ -19060,6 +20056,9 @@
       <c r="C81">
         <v>2.4557259999999999</v>
       </c>
+      <c r="E81">
+        <v>6.1765E-2</v>
+      </c>
       <c r="S81">
         <v>128</v>
       </c>
@@ -19068,6 +20067,9 @@
       </c>
       <c r="U81">
         <v>0.22631200000000001</v>
+      </c>
+      <c r="W81">
+        <v>5.9046000000000001E-2</v>
       </c>
     </row>
     <row r="82" spans="1:24" x14ac:dyDescent="0.25">
@@ -19080,6 +20082,9 @@
       <c r="C82">
         <v>6.4684039999999996</v>
       </c>
+      <c r="E82">
+        <v>0.16472999999999999</v>
+      </c>
       <c r="S82">
         <v>256</v>
       </c>
@@ -19088,6 +20093,9 @@
       </c>
       <c r="U82">
         <v>0.46893299999999999</v>
+      </c>
+      <c r="W82">
+        <v>0.13297500000000001</v>
       </c>
     </row>
     <row r="84" spans="1:24" x14ac:dyDescent="0.25">
@@ -19138,6 +20146,9 @@
       <c r="C85">
         <v>3.5201000000000003E-2</v>
       </c>
+      <c r="E85">
+        <v>2.7614E-2</v>
+      </c>
       <c r="S85">
         <v>8</v>
       </c>
@@ -19146,6 +20157,9 @@
       </c>
       <c r="U85">
         <v>4.4990000000000004E-3</v>
+      </c>
+      <c r="W85">
+        <v>2.5940000000000001E-2</v>
       </c>
     </row>
     <row r="86" spans="1:24" x14ac:dyDescent="0.25">
@@ -19158,6 +20172,9 @@
       <c r="C86">
         <v>4.6632E-2</v>
       </c>
+      <c r="E86">
+        <v>2.9433999999999998E-2</v>
+      </c>
       <c r="S86">
         <v>16</v>
       </c>
@@ -19166,6 +20183,9 @@
       </c>
       <c r="U86">
         <v>3.3969999999999998E-3</v>
+      </c>
+      <c r="W86">
+        <v>2.8344999999999999E-2</v>
       </c>
     </row>
     <row r="87" spans="1:24" x14ac:dyDescent="0.25">
@@ -19178,6 +20198,9 @@
       <c r="C87">
         <v>4.8320000000000002E-2</v>
       </c>
+      <c r="E87">
+        <v>4.6836000000000003E-2</v>
+      </c>
       <c r="S87">
         <v>32</v>
       </c>
@@ -19186,6 +20209,9 @@
       </c>
       <c r="U87">
         <v>2.9420000000000002E-3</v>
+      </c>
+      <c r="W87">
+        <v>4.5185000000000003E-2</v>
       </c>
     </row>
     <row r="88" spans="1:24" x14ac:dyDescent="0.25">
@@ -19198,6 +20224,9 @@
       <c r="C88">
         <v>3.2274999999999998E-2</v>
       </c>
+      <c r="E88">
+        <v>3.4745999999999999E-2</v>
+      </c>
       <c r="S88">
         <v>64</v>
       </c>
@@ -19206,6 +20235,9 @@
       </c>
       <c r="U88">
         <v>5.2700000000000004E-3</v>
+      </c>
+      <c r="W88">
+        <v>3.4556000000000003E-2</v>
       </c>
     </row>
     <row r="89" spans="1:24" x14ac:dyDescent="0.25">
@@ -19218,6 +20250,9 @@
       <c r="C89">
         <v>2.3438979999999998</v>
       </c>
+      <c r="E89">
+        <v>6.5581E-2</v>
+      </c>
       <c r="S89">
         <v>128</v>
       </c>
@@ -19226,6 +20261,9 @@
       </c>
       <c r="U89">
         <v>0.161133</v>
+      </c>
+      <c r="W89">
+        <v>6.0690000000000001E-2</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
@@ -19238,6 +20276,9 @@
       <c r="C90">
         <v>7.209714</v>
       </c>
+      <c r="E90">
+        <v>0.16339799999999999</v>
+      </c>
       <c r="S90">
         <v>256</v>
       </c>
@@ -19246,6 +20287,9 @@
       </c>
       <c r="U90">
         <v>0.87797199999999997</v>
+      </c>
+      <c r="W90">
+        <v>0.160995</v>
       </c>
     </row>
     <row r="92" spans="1:24" x14ac:dyDescent="0.25">
@@ -19296,6 +20340,9 @@
       <c r="C93">
         <v>0.20039499999999999</v>
       </c>
+      <c r="E93">
+        <v>9.9562999999999999E-2</v>
+      </c>
       <c r="S93">
         <v>8</v>
       </c>
@@ -19304,6 +20351,9 @@
       </c>
       <c r="U93">
         <v>2.443E-2</v>
+      </c>
+      <c r="W93">
+        <v>8.9981000000000005E-2</v>
       </c>
     </row>
     <row r="94" spans="1:24" x14ac:dyDescent="0.25">
@@ -19316,6 +20366,9 @@
       <c r="C94">
         <v>0.189828</v>
       </c>
+      <c r="E94">
+        <v>9.2874999999999999E-2</v>
+      </c>
       <c r="S94">
         <v>16</v>
       </c>
@@ -19324,6 +20377,9 @@
       </c>
       <c r="U94">
         <v>1.4648E-2</v>
+      </c>
+      <c r="W94">
+        <v>8.8151999999999994E-2</v>
       </c>
     </row>
     <row r="95" spans="1:24" x14ac:dyDescent="0.25">
@@ -19336,6 +20392,9 @@
       <c r="C95">
         <v>0.20424300000000001</v>
       </c>
+      <c r="E95">
+        <v>0.109123</v>
+      </c>
       <c r="S95">
         <v>32</v>
       </c>
@@ -19344,6 +20403,9 @@
       </c>
       <c r="U95">
         <v>9.6629999999999997E-3</v>
+      </c>
+      <c r="W95">
+        <v>9.1856999999999994E-2</v>
       </c>
     </row>
     <row r="96" spans="1:24" x14ac:dyDescent="0.25">
@@ -19356,6 +20418,9 @@
       <c r="C96">
         <v>0.19129499999999999</v>
       </c>
+      <c r="E96">
+        <v>0.16328699999999999</v>
+      </c>
       <c r="S96">
         <v>64</v>
       </c>
@@ -19364,6 +20429,9 @@
       </c>
       <c r="U96">
         <v>8.4489999999999999E-3</v>
+      </c>
+      <c r="W96">
+        <v>0.16197600000000001</v>
       </c>
     </row>
     <row r="97" spans="1:24" x14ac:dyDescent="0.25">
@@ -19376,6 +20444,9 @@
       <c r="C97">
         <v>2.5127320000000002</v>
       </c>
+      <c r="E97">
+        <v>0.183536</v>
+      </c>
       <c r="S97">
         <v>128</v>
       </c>
@@ -19384,6 +20455,9 @@
       </c>
       <c r="U97">
         <v>0.49077300000000001</v>
+      </c>
+      <c r="W97">
+        <v>0.170323</v>
       </c>
     </row>
     <row r="98" spans="1:24" x14ac:dyDescent="0.25">
@@ -19396,6 +20470,9 @@
       <c r="C98">
         <v>7.0089990000000002</v>
       </c>
+      <c r="E98">
+        <v>0.46755000000000002</v>
+      </c>
       <c r="S98">
         <v>256</v>
       </c>
@@ -19404,6 +20481,9 @@
       </c>
       <c r="U98">
         <v>0.24757499999999999</v>
+      </c>
+      <c r="W98">
+        <v>0.46067200000000003</v>
       </c>
     </row>
     <row r="100" spans="1:24" x14ac:dyDescent="0.25">
@@ -19466,6 +20546,9 @@
       <c r="U102">
         <v>2.0306000000000001E-2</v>
       </c>
+      <c r="W102">
+        <v>3.6999999999999998E-5</v>
+      </c>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A103">
@@ -19486,6 +20569,9 @@
       <c r="U103">
         <v>2.8608999999999999E-2</v>
       </c>
+      <c r="W103">
+        <v>2.6999999999999999E-5</v>
+      </c>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A104">
@@ -19506,6 +20592,9 @@
       <c r="U104">
         <v>3.5257999999999998E-2</v>
       </c>
+      <c r="W104">
+        <v>1.8E-5</v>
+      </c>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A105">
@@ -19526,6 +20615,9 @@
       <c r="U105">
         <v>3.0117000000000001E-2</v>
       </c>
+      <c r="W105">
+        <v>1.5E-5</v>
+      </c>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A106">
@@ -19546,6 +20638,9 @@
       <c r="U106">
         <v>2.0979890000000001</v>
       </c>
+      <c r="W106">
+        <v>6.9999999999999999E-6</v>
+      </c>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A107">
@@ -19566,6 +20661,9 @@
       <c r="U107">
         <v>5.9382239999999999</v>
       </c>
+      <c r="W107">
+        <v>7.9999999999999996E-6</v>
+      </c>
     </row>
     <row r="109" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -19615,6 +20713,9 @@
       <c r="U110">
         <v>1.8815999999999999E-2</v>
       </c>
+      <c r="W110">
+        <v>2.7399999999999999E-4</v>
+      </c>
     </row>
     <row r="111" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A111">
@@ -19635,6 +20736,9 @@
       <c r="U111">
         <v>1.4069999999999999E-2</v>
       </c>
+      <c r="W111">
+        <v>1.36E-4</v>
+      </c>
     </row>
     <row r="112" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A112">
@@ -19655,6 +20759,9 @@
       <c r="U112">
         <v>1.8197999999999999E-2</v>
       </c>
+      <c r="W112">
+        <v>8.2000000000000001E-5</v>
+      </c>
     </row>
     <row r="113" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A113">
@@ -19675,6 +20782,9 @@
       <c r="U113">
         <v>2.367E-2</v>
       </c>
+      <c r="W113">
+        <v>4.6999999999999997E-5</v>
+      </c>
     </row>
     <row r="114" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A114">
@@ -19695,6 +20805,9 @@
       <c r="U114">
         <v>1.9417420000000001</v>
       </c>
+      <c r="W114">
+        <v>3.6999999999999998E-5</v>
+      </c>
     </row>
     <row r="115" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A115">
@@ -19715,6 +20828,9 @@
       <c r="U115">
         <v>5.6845189999999999</v>
       </c>
+      <c r="W115">
+        <v>1.12E-4</v>
+      </c>
     </row>
     <row r="117" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -19764,6 +20880,9 @@
       <c r="U118">
         <v>3.1274999999999997E-2</v>
       </c>
+      <c r="W118">
+        <v>3.3909999999999999E-3</v>
+      </c>
     </row>
     <row r="119" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A119">
@@ -19784,6 +20903,9 @@
       <c r="U119">
         <v>4.1695000000000003E-2</v>
       </c>
+      <c r="W119">
+        <v>1.555E-3</v>
+      </c>
     </row>
     <row r="120" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A120">
@@ -19804,6 +20926,9 @@
       <c r="U120">
         <v>5.8226E-2</v>
       </c>
+      <c r="W120">
+        <v>7.1299999999999998E-4</v>
+      </c>
     </row>
     <row r="121" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A121">
@@ -19824,6 +20949,9 @@
       <c r="U121">
         <v>4.1966000000000003E-2</v>
       </c>
+      <c r="W121">
+        <v>3.6099999999999999E-4</v>
+      </c>
     </row>
     <row r="122" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A122">
@@ -19844,6 +20972,9 @@
       <c r="U122">
         <v>2.2604609999999998</v>
       </c>
+      <c r="W122">
+        <v>1.8699999999999999E-4</v>
+      </c>
     </row>
     <row r="123" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A123">
@@ -19864,6 +20995,9 @@
       <c r="U123">
         <v>5.6838110000000004</v>
       </c>
+      <c r="W123">
+        <v>8.7000000000000001E-5</v>
+      </c>
     </row>
     <row r="125" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -19913,6 +21047,9 @@
       <c r="U126">
         <v>0.271144</v>
       </c>
+      <c r="W126">
+        <v>3.6357E-2</v>
+      </c>
     </row>
     <row r="127" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A127">
@@ -19933,6 +21070,9 @@
       <c r="U127">
         <v>0.242871</v>
       </c>
+      <c r="W127">
+        <v>1.7686E-2</v>
+      </c>
     </row>
     <row r="128" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A128">
@@ -19953,6 +21093,9 @@
       <c r="U128">
         <v>0.26889299999999999</v>
       </c>
+      <c r="W128">
+        <v>8.7899999999999992E-3</v>
+      </c>
     </row>
     <row r="129" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A129">
@@ -19973,6 +21116,9 @@
       <c r="U129">
         <v>0.189412</v>
       </c>
+      <c r="W129">
+        <v>3.9379999999999997E-3</v>
+      </c>
     </row>
     <row r="130" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A130">
@@ -19993,6 +21139,9 @@
       <c r="U130">
         <v>1.8458049999999999</v>
       </c>
+      <c r="W130">
+        <v>2.215E-3</v>
+      </c>
     </row>
     <row r="131" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A131">
@@ -20012,6 +21161,9 @@
       </c>
       <c r="U131">
         <v>6.5948310000000001</v>
+      </c>
+      <c r="W131">
+        <v>1.3749999999999999E-3</v>
       </c>
     </row>
     <row r="133" spans="1:24" x14ac:dyDescent="0.25">
@@ -20051,6 +21203,9 @@
       <c r="U135">
         <v>2.1472000000000002E-2</v>
       </c>
+      <c r="W135">
+        <v>2.0999999999999999E-5</v>
+      </c>
     </row>
     <row r="136" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S136">
@@ -20062,6 +21217,9 @@
       <c r="U136">
         <v>2.3215E-2</v>
       </c>
+      <c r="W136">
+        <v>2.6999999999999999E-5</v>
+      </c>
     </row>
     <row r="137" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S137">
@@ -20073,6 +21231,9 @@
       <c r="U137">
         <v>3.4338E-2</v>
       </c>
+      <c r="W137">
+        <v>2.5000000000000001E-5</v>
+      </c>
     </row>
     <row r="138" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S138">
@@ -20084,6 +21245,9 @@
       <c r="U138">
         <v>1.269E-2</v>
       </c>
+      <c r="W138">
+        <v>1.8E-5</v>
+      </c>
     </row>
     <row r="139" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S139">
@@ -20095,6 +21259,9 @@
       <c r="U139">
         <v>2.2542270000000002</v>
       </c>
+      <c r="W139">
+        <v>8.5000000000000006E-5</v>
+      </c>
     </row>
     <row r="140" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S140">
@@ -20106,6 +21273,9 @@
       <c r="U140">
         <v>6.6103699999999996</v>
       </c>
+      <c r="W140">
+        <v>6.0000000000000002E-6</v>
+      </c>
     </row>
     <row r="142" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S142" t="s">
@@ -20137,6 +21307,9 @@
       <c r="U143">
         <v>2.0059E-2</v>
       </c>
+      <c r="W143">
+        <v>8.2999999999999998E-5</v>
+      </c>
     </row>
     <row r="144" spans="1:24" x14ac:dyDescent="0.25">
       <c r="S144">
@@ -20148,6 +21321,9 @@
       <c r="U144">
         <v>1.3467E-2</v>
       </c>
+      <c r="W144">
+        <v>5.0000000000000002E-5</v>
+      </c>
     </row>
     <row r="145" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S145">
@@ -20159,6 +21335,9 @@
       <c r="U145">
         <v>4.0439000000000003E-2</v>
       </c>
+      <c r="W145">
+        <v>3.0000000000000001E-5</v>
+      </c>
     </row>
     <row r="146" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S146">
@@ -20170,6 +21349,9 @@
       <c r="U146">
         <v>1.6976000000000002E-2</v>
       </c>
+      <c r="W146">
+        <v>2.5999999999999998E-5</v>
+      </c>
     </row>
     <row r="147" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S147">
@@ -20181,6 +21363,9 @@
       <c r="U147">
         <v>2.2544420000000001</v>
       </c>
+      <c r="W147">
+        <v>1.8E-5</v>
+      </c>
     </row>
     <row r="148" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S148">
@@ -20192,6 +21377,9 @@
       <c r="U148">
         <v>5.570926</v>
       </c>
+      <c r="W148">
+        <v>5.3999999999999998E-5</v>
+      </c>
     </row>
     <row r="150" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S150" t="s">
@@ -20223,6 +21411,9 @@
       <c r="U151">
         <v>2.7980000000000001E-2</v>
       </c>
+      <c r="W151">
+        <v>7.0799999999999997E-4</v>
+      </c>
     </row>
     <row r="152" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S152">
@@ -20234,6 +21425,9 @@
       <c r="U152">
         <v>3.7458999999999999E-2</v>
       </c>
+      <c r="W152">
+        <v>3.8699999999999997E-4</v>
+      </c>
     </row>
     <row r="153" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S153">
@@ -20245,6 +21439,9 @@
       <c r="U153">
         <v>5.2458999999999999E-2</v>
       </c>
+      <c r="W153">
+        <v>1.92E-4</v>
+      </c>
     </row>
     <row r="154" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S154">
@@ -20256,6 +21453,9 @@
       <c r="U154">
         <v>3.5234000000000001E-2</v>
       </c>
+      <c r="W154">
+        <v>1.08E-4</v>
+      </c>
     </row>
     <row r="155" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S155">
@@ -20267,6 +21467,9 @@
       <c r="U155">
         <v>2.194766</v>
       </c>
+      <c r="W155">
+        <v>5.3000000000000001E-5</v>
+      </c>
     </row>
     <row r="156" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S156">
@@ -20278,6 +21481,9 @@
       <c r="U156">
         <v>5.9706010000000003</v>
       </c>
+      <c r="W156">
+        <v>3.4E-5</v>
+      </c>
     </row>
     <row r="158" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S158" t="s">
@@ -20309,6 +21515,9 @@
       <c r="U159">
         <v>0.201681</v>
       </c>
+      <c r="W159">
+        <v>8.3829999999999998E-3</v>
+      </c>
     </row>
     <row r="160" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S160">
@@ -20320,6 +21529,9 @@
       <c r="U160">
         <v>0.201208</v>
       </c>
+      <c r="W160">
+        <v>3.823E-3</v>
+      </c>
     </row>
     <row r="161" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S161">
@@ -20331,6 +21543,9 @@
       <c r="U161">
         <v>0.26687100000000002</v>
       </c>
+      <c r="W161">
+        <v>1.853E-3</v>
+      </c>
     </row>
     <row r="162" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S162">
@@ -20342,6 +21557,9 @@
       <c r="U162">
         <v>0.193</v>
       </c>
+      <c r="W162">
+        <v>9.0799999999999995E-4</v>
+      </c>
     </row>
     <row r="163" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S163">
@@ -20353,6 +21571,9 @@
       <c r="U163">
         <v>2.237479</v>
       </c>
+      <c r="W163">
+        <v>6.1600000000000001E-4</v>
+      </c>
     </row>
     <row r="164" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S164">
@@ -20363,6 +21584,9 @@
       </c>
       <c r="U164">
         <v>6.8253950000000003</v>
+      </c>
+      <c r="W164">
+        <v>2.4899999999999998E-4</v>
       </c>
     </row>
     <row r="166" spans="19:24" x14ac:dyDescent="0.25">
@@ -20402,6 +21626,9 @@
       <c r="U168">
         <v>1.4822999999999999E-2</v>
       </c>
+      <c r="W168">
+        <v>2.4000000000000001E-5</v>
+      </c>
     </row>
     <row r="169" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S169">
@@ -20413,6 +21640,9 @@
       <c r="U169">
         <v>4.0251000000000002E-2</v>
       </c>
+      <c r="W169">
+        <v>2.5000000000000001E-5</v>
+      </c>
     </row>
     <row r="170" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S170">
@@ -20424,6 +21654,9 @@
       <c r="U170">
         <v>3.0113999999999998E-2</v>
       </c>
+      <c r="W170">
+        <v>1.5999999999999999E-5</v>
+      </c>
     </row>
     <row r="171" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S171">
@@ -20435,6 +21668,9 @@
       <c r="U171">
         <v>2.0611999999999998E-2</v>
       </c>
+      <c r="W171">
+        <v>1.4E-5</v>
+      </c>
     </row>
     <row r="172" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S172">
@@ -20446,6 +21682,9 @@
       <c r="U172">
         <v>2.2623150000000001</v>
       </c>
+      <c r="W172">
+        <v>6.4999999999999994E-5</v>
+      </c>
     </row>
     <row r="173" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S173">
@@ -20457,6 +21696,9 @@
       <c r="U173">
         <v>6.4998820000000004</v>
       </c>
+      <c r="W173">
+        <v>6.0000000000000002E-6</v>
+      </c>
     </row>
     <row r="175" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S175" t="s">
@@ -20488,6 +21730,9 @@
       <c r="U176">
         <v>2.112E-2</v>
       </c>
+      <c r="W176">
+        <v>7.7999999999999999E-5</v>
+      </c>
     </row>
     <row r="177" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S177">
@@ -20499,6 +21744,9 @@
       <c r="U177">
         <v>2.1204000000000001E-2</v>
       </c>
+      <c r="W177">
+        <v>4.6E-5</v>
+      </c>
     </row>
     <row r="178" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S178">
@@ -20510,6 +21758,9 @@
       <c r="U178">
         <v>3.9477999999999999E-2</v>
       </c>
+      <c r="W178">
+        <v>3.8000000000000002E-5</v>
+      </c>
     </row>
     <row r="179" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S179">
@@ -20521,6 +21772,9 @@
       <c r="U179">
         <v>4.2495999999999999E-2</v>
       </c>
+      <c r="W179">
+        <v>2.9E-5</v>
+      </c>
     </row>
     <row r="180" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S180">
@@ -20532,6 +21786,9 @@
       <c r="U180">
         <v>2.2290999999999999</v>
       </c>
+      <c r="W180">
+        <v>1.8E-5</v>
+      </c>
     </row>
     <row r="181" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S181">
@@ -20543,6 +21800,9 @@
       <c r="U181">
         <v>6.01295</v>
       </c>
+      <c r="W181">
+        <v>1.5999999999999999E-5</v>
+      </c>
     </row>
     <row r="183" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S183" t="s">
@@ -20574,6 +21834,9 @@
       <c r="U184">
         <v>3.5316E-2</v>
       </c>
+      <c r="W184">
+        <v>7.3499999999999998E-4</v>
+      </c>
     </row>
     <row r="185" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S185">
@@ -20585,6 +21848,9 @@
       <c r="U185">
         <v>4.5884000000000001E-2</v>
       </c>
+      <c r="W185">
+        <v>3.8299999999999999E-4</v>
+      </c>
     </row>
     <row r="186" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S186">
@@ -20596,6 +21862,9 @@
       <c r="U186">
         <v>4.3895000000000003E-2</v>
       </c>
+      <c r="W186">
+        <v>2.0000000000000001E-4</v>
+      </c>
     </row>
     <row r="187" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S187">
@@ -20607,6 +21876,9 @@
       <c r="U187">
         <v>3.0352000000000001E-2</v>
       </c>
+      <c r="W187">
+        <v>1.1E-4</v>
+      </c>
     </row>
     <row r="188" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S188">
@@ -20618,6 +21890,9 @@
       <c r="U188">
         <v>2.1592880000000001</v>
       </c>
+      <c r="W188">
+        <v>5.3999999999999998E-5</v>
+      </c>
     </row>
     <row r="189" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S189">
@@ -20629,6 +21904,9 @@
       <c r="U189">
         <v>6.7297859999999998</v>
       </c>
+      <c r="W189">
+        <v>3.4999999999999997E-5</v>
+      </c>
     </row>
     <row r="191" spans="19:24" x14ac:dyDescent="0.25">
       <c r="S191" t="s">
@@ -20660,8 +21938,11 @@
       <c r="U192">
         <v>0.19377800000000001</v>
       </c>
+      <c r="W192">
+        <v>8.2019999999999992E-3</v>
+      </c>
     </row>
-    <row r="193" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="193" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S193">
         <v>16</v>
       </c>
@@ -20671,8 +21952,11 @@
       <c r="U193">
         <v>0.18944</v>
       </c>
+      <c r="W193">
+        <v>4.0340000000000003E-3</v>
+      </c>
     </row>
-    <row r="194" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="194" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S194">
         <v>32</v>
       </c>
@@ -20682,8 +21966,11 @@
       <c r="U194">
         <v>0.20013300000000001</v>
       </c>
+      <c r="W194">
+        <v>2.1510000000000001E-3</v>
+      </c>
     </row>
-    <row r="195" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="195" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S195">
         <v>64</v>
       </c>
@@ -20693,8 +21980,11 @@
       <c r="U195">
         <v>0.17430899999999999</v>
       </c>
+      <c r="W195">
+        <v>1.3209999999999999E-3</v>
+      </c>
     </row>
-    <row r="196" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="196" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S196">
         <v>128</v>
       </c>
@@ -20704,8 +21994,11 @@
       <c r="U196">
         <v>2.2697859999999999</v>
       </c>
+      <c r="W196">
+        <v>6.0700000000000001E-4</v>
+      </c>
     </row>
-    <row r="197" spans="19:21" x14ac:dyDescent="0.25">
+    <row r="197" spans="19:23" x14ac:dyDescent="0.25">
       <c r="S197">
         <v>256</v>
       </c>
@@ -20714,6 +22007,9 @@
       </c>
       <c r="U197">
         <v>6.0941890000000001</v>
+      </c>
+      <c r="W197">
+        <v>4.1800000000000002E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added quicksort data to sheet
</commit_message>
<xml_diff>
--- a/all_data.xlsx
+++ b/all_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\siraius\Class_Files\CSCE435\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vicen\Documents\csce435project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{520B9147-0D0C-48B9-ABA5-C7148FB81A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3DCFCF-2B99-4753-9833-4139C98E1D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7200" yWindow="540" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Compiled Data" sheetId="4" r:id="rId1"/>
@@ -119,7 +119,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,13 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444444"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -156,12 +163,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,6 +539,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2364E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.5451999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5409999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9475999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4493999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.9265000000000006E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -695,6 +721,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.2113000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.7952000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6509E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.0080000000000004E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.9593999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11887399999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -863,6 +907,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4649000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0048E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.4432999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4043999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10717500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.118177</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1035,6 +1097,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.11228399999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8349999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.111779</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12899099999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28734300000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.443963</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1704,6 +1784,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.1310000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0429999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.7390000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6081999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.2253000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.1018000000000002E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1868,6 +1966,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.1221E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.2329999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.545E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5004999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.4911999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.121527</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2036,6 +2152,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.3099999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9.7040000000000008E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8169999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8797999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3127000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.153255</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2208,6 +2342,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.2034E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0501E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7268000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4879E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5350999999999996E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.17979700000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -5908,6 +6060,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.2950000000000002E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9459000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3668999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0011999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7289E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3159000000000007E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6072,6 +6242,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.1473000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.8052000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2391999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.2779999999999997E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.3997999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3769000000000006E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6240,6 +6428,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3.4338E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7707000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0133000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3820999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.8272000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2777000000000003E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -6412,6 +6618,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.9216E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.4427999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0640000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.6342000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.4229000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.104893</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7081,6 +7305,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.5719999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0250000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.1577000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2010999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1776E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.8702999999999995E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7245,6 +7487,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6642000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8213E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.7397E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2160000000000001E-3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5702E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.0645999999999999E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7413,6 +7673,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.3943000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8565999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8176E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2918000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4602000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.8957000000000003E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -7585,6 +7863,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.104E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.6762000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.6427000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6237999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1371000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.101713</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8254,6 +8550,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.8674E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.1913999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9567000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6893E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.1139999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.3352E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8418,6 +8732,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6182999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0408999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7456000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.3357999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.7145999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.0359999999999997E-3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8586,6 +8918,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.5610000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8679000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.945E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2832E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5725000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.14138800000000001</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -8758,6 +9108,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.787E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2416E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2516000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.6624999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7829E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.153311</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9427,6 +9795,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.5932000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.7932E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.605E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.2580999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.3001000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.9913000000000007E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9591,6 +9977,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.8329999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.4019E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3931000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5627E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4365999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.5460999999999999E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9759,6 +10163,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4937000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.3643999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.8670000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.9288999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.10155500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1212000000000006E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -9931,6 +10353,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.7901E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.3878999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6337000000000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.32E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.4585999999999995E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16179099999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10600,6 +11040,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.8436999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2390999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.3266999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2478E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.1126999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.1311999999999995E-2</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10764,6 +11222,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.2051999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2297000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0191E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9289000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.3955999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13647699999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -10932,6 +11408,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4508999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.6212000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.2460999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.524E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.3803000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.15889</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -11104,6 +11598,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.1561E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.8799E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.0637E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.2352000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5550000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.157607</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -12459,6 +12971,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.175E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.9789999999999991E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.6871000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.1998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1069999999999997E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.135628</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -12731,6 +13261,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.4549999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9907000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1572999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.2851E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.2641999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.116288</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13007,6 +13555,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.0068000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.7519999999999994E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3837E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.6997999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.5725000000000006E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.165934</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13287,6 +13853,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.4394000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.1939999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.9265000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3268E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7829E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.145428</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -13956,6 +14540,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.7590000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5329999999999998E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0697999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.5703999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.2245000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.103587</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14228,6 +14830,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.8669999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.293E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.0530000000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4133E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1854000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.108679</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14504,6 +15124,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.5989999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6519999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0392E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.0022999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1121000000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.11643199999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -14784,6 +15422,24 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.2959999999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.9436999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.1850000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4317E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.2733000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16811899999999999</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -23507,36 +24163,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB7B859C-9CEF-4DEA-AF23-94F3B0B7BC2A}">
   <dimension ref="A1:X197"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O160" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T204" sqref="T204"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2:X197"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" customWidth="1"/>
-    <col min="4" max="5" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.42578125" customWidth="1"/>
-    <col min="22" max="22" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="5" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.44140625" customWidth="1"/>
+    <col min="22" max="22" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="S1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="S1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -23574,7 +24230,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>8</v>
       </c>
@@ -23587,6 +24243,9 @@
       <c r="E3">
         <v>5.8869999999999999E-3</v>
       </c>
+      <c r="F3" s="3">
+        <v>1.2364E-2</v>
+      </c>
       <c r="S3">
         <v>8</v>
       </c>
@@ -23599,8 +24258,11 @@
       <c r="W3">
         <v>5.4380000000000001E-3</v>
       </c>
+      <c r="X3">
+        <v>1.8674E-2</v>
+      </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>16</v>
       </c>
@@ -23613,6 +24275,9 @@
       <c r="E4">
         <v>1.8318000000000001E-2</v>
       </c>
+      <c r="F4" s="3">
+        <v>2.5451999999999999E-2</v>
+      </c>
       <c r="S4">
         <v>16</v>
       </c>
@@ -23625,8 +24290,11 @@
       <c r="W4">
         <v>1.7894E-2</v>
       </c>
+      <c r="X4">
+        <v>2.1913999999999999E-2</v>
+      </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>32</v>
       </c>
@@ -23639,6 +24307,9 @@
       <c r="E5">
         <v>4.0058999999999997E-2</v>
       </c>
+      <c r="F5" s="3">
+        <v>4.5409999999999999E-2</v>
+      </c>
       <c r="S5">
         <v>32</v>
       </c>
@@ -23651,8 +24322,11 @@
       <c r="W5">
         <v>3.9638E-2</v>
       </c>
+      <c r="X5">
+        <v>1.9567000000000001E-2</v>
+      </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>64</v>
       </c>
@@ -23665,6 +24339,9 @@
       <c r="E6">
         <v>1.6011000000000001E-2</v>
       </c>
+      <c r="F6" s="3">
+        <v>2.9475999999999999E-2</v>
+      </c>
       <c r="S6">
         <v>64</v>
       </c>
@@ -23677,8 +24354,11 @@
       <c r="W6">
         <v>1.5611999999999999E-2</v>
       </c>
+      <c r="X6">
+        <v>2.6893E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>128</v>
       </c>
@@ -23691,6 +24371,9 @@
       <c r="E7">
         <v>9.3562999999999993E-2</v>
       </c>
+      <c r="F7" s="3">
+        <v>6.4493999999999996E-2</v>
+      </c>
       <c r="S7">
         <v>128</v>
       </c>
@@ -23703,8 +24386,11 @@
       <c r="W7">
         <v>7.9904000000000003E-2</v>
       </c>
+      <c r="X7">
+        <v>2.1139999999999999E-2</v>
+      </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>256</v>
       </c>
@@ -23717,6 +24403,9 @@
       <c r="E8">
         <v>0.34959099999999999</v>
       </c>
+      <c r="F8" s="3">
+        <v>9.9265000000000006E-2</v>
+      </c>
       <c r="S8">
         <v>256</v>
       </c>
@@ -23729,8 +24418,11 @@
       <c r="W8">
         <v>0.32938699999999999</v>
       </c>
+      <c r="X8">
+        <v>3.3352E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -23768,7 +24460,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8</v>
       </c>
@@ -23781,6 +24473,9 @@
       <c r="E11">
         <v>1.4194E-2</v>
       </c>
+      <c r="F11" s="3">
+        <v>2.2113000000000001E-2</v>
+      </c>
       <c r="S11">
         <v>8</v>
       </c>
@@ -23793,8 +24488,11 @@
       <c r="W11">
         <v>1.3442000000000001E-2</v>
       </c>
+      <c r="X11">
+        <v>1.6182999999999999E-2</v>
+      </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>16</v>
       </c>
@@ -23807,6 +24505,9 @@
       <c r="E12">
         <v>2.4081999999999999E-2</v>
       </c>
+      <c r="F12" s="3">
+        <v>2.7952000000000001E-2</v>
+      </c>
       <c r="S12">
         <v>16</v>
       </c>
@@ -23819,8 +24520,11 @@
       <c r="W12">
         <v>2.3601E-2</v>
       </c>
+      <c r="X12">
+        <v>3.0408999999999999E-2</v>
+      </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>32</v>
       </c>
@@ -23833,6 +24537,9 @@
       <c r="E13">
         <v>4.2880000000000001E-2</v>
       </c>
+      <c r="F13" s="3">
+        <v>3.6509E-2</v>
+      </c>
       <c r="S13">
         <v>32</v>
       </c>
@@ -23845,8 +24552,11 @@
       <c r="W13">
         <v>4.2437000000000002E-2</v>
       </c>
+      <c r="X13">
+        <v>2.7456000000000001E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>64</v>
       </c>
@@ -23859,6 +24569,9 @@
       <c r="E14">
         <v>4.0288999999999998E-2</v>
       </c>
+      <c r="F14" s="3">
+        <v>9.0080000000000004E-3</v>
+      </c>
       <c r="S14">
         <v>64</v>
       </c>
@@ -23871,8 +24584,11 @@
       <c r="W14">
         <v>3.9740999999999999E-2</v>
       </c>
+      <c r="X14">
+        <v>3.3357999999999999E-2</v>
+      </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>128</v>
       </c>
@@ -23885,6 +24601,9 @@
       <c r="E15">
         <v>7.1009000000000003E-2</v>
       </c>
+      <c r="F15" s="3">
+        <v>7.9593999999999998E-2</v>
+      </c>
       <c r="S15">
         <v>128</v>
       </c>
@@ -23897,8 +24616,11 @@
       <c r="W15">
         <v>6.8210999999999994E-2</v>
       </c>
+      <c r="X15">
+        <v>3.7145999999999998E-2</v>
+      </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>256</v>
       </c>
@@ -23911,6 +24633,9 @@
       <c r="E16">
         <v>0.112997</v>
       </c>
+      <c r="F16" s="3">
+        <v>0.11887399999999999</v>
+      </c>
       <c r="S16">
         <v>256</v>
       </c>
@@ -23923,8 +24648,11 @@
       <c r="W16">
         <v>0.10834000000000001</v>
       </c>
+      <c r="X16">
+        <v>5.0359999999999997E-3</v>
+      </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -23962,7 +24690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>8</v>
       </c>
@@ -23975,6 +24703,9 @@
       <c r="E19">
         <v>3.1519999999999999E-2</v>
       </c>
+      <c r="F19" s="3">
+        <v>1.4649000000000001E-2</v>
+      </c>
       <c r="S19">
         <v>8</v>
       </c>
@@ -23987,8 +24718,11 @@
       <c r="W19">
         <v>2.7518999999999998E-2</v>
       </c>
+      <c r="X19">
+        <v>2.5610000000000001E-2</v>
+      </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>16</v>
       </c>
@@ -24001,6 +24735,9 @@
       <c r="E20">
         <v>3.1215E-2</v>
       </c>
+      <c r="F20" s="3">
+        <v>2.0048E-2</v>
+      </c>
       <c r="S20">
         <v>16</v>
       </c>
@@ -24013,8 +24750,11 @@
       <c r="W20">
         <v>2.9149000000000001E-2</v>
       </c>
+      <c r="X20">
+        <v>1.8679000000000001E-2</v>
+      </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>32</v>
       </c>
@@ -24027,6 +24767,9 @@
       <c r="E21">
         <v>6.0942000000000003E-2</v>
       </c>
+      <c r="F21" s="3">
+        <v>3.4432999999999998E-2</v>
+      </c>
       <c r="S21">
         <v>32</v>
       </c>
@@ -24039,8 +24782,11 @@
       <c r="W21">
         <v>5.9187999999999998E-2</v>
       </c>
+      <c r="X21">
+        <v>2.945E-2</v>
+      </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>64</v>
       </c>
@@ -24053,6 +24799,9 @@
       <c r="E22">
         <v>2.8743000000000001E-2</v>
       </c>
+      <c r="F22" s="3">
+        <v>3.4043999999999998E-2</v>
+      </c>
       <c r="S22">
         <v>64</v>
       </c>
@@ -24065,8 +24814,11 @@
       <c r="W22">
         <v>2.802E-2</v>
       </c>
+      <c r="X22">
+        <v>3.2832E-2</v>
+      </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>128</v>
       </c>
@@ -24079,6 +24831,9 @@
       <c r="E23">
         <v>7.9242999999999994E-2</v>
       </c>
+      <c r="F23" s="3">
+        <v>0.10717500000000001</v>
+      </c>
       <c r="S23">
         <v>128</v>
       </c>
@@ -24091,8 +24846,11 @@
       <c r="W23">
         <v>7.5854000000000005E-2</v>
       </c>
+      <c r="X23">
+        <v>6.5725000000000006E-2</v>
+      </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>256</v>
       </c>
@@ -24105,6 +24863,9 @@
       <c r="E24">
         <v>9.8211000000000007E-2</v>
       </c>
+      <c r="F24" s="3">
+        <v>0.118177</v>
+      </c>
       <c r="S24">
         <v>256</v>
       </c>
@@ -24117,8 +24878,11 @@
       <c r="W24">
         <v>9.8047999999999996E-2</v>
       </c>
+      <c r="X24">
+        <v>0.14138800000000001</v>
+      </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -24156,7 +24920,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>8</v>
       </c>
@@ -24169,6 +24933,9 @@
       <c r="E27">
         <v>0.15631900000000001</v>
       </c>
+      <c r="F27" s="3">
+        <v>0.11228399999999999</v>
+      </c>
       <c r="S27">
         <v>8</v>
       </c>
@@ -24181,8 +24948,11 @@
       <c r="W27">
         <v>0.11808100000000001</v>
       </c>
+      <c r="X27">
+        <v>1.787E-3</v>
+      </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>16</v>
       </c>
@@ -24195,6 +24965,9 @@
       <c r="E28">
         <v>0.15681400000000001</v>
       </c>
+      <c r="F28" s="3">
+        <v>8.8349999999999998E-2</v>
+      </c>
       <c r="S28">
         <v>16</v>
       </c>
@@ -24207,8 +24980,11 @@
       <c r="W28">
         <v>0.138021</v>
       </c>
+      <c r="X28">
+        <v>1.2416E-2</v>
+      </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>32</v>
       </c>
@@ -24221,6 +24997,9 @@
       <c r="E29">
         <v>0.168438</v>
       </c>
+      <c r="F29" s="3">
+        <v>0.111779</v>
+      </c>
       <c r="S29">
         <v>32</v>
       </c>
@@ -24233,8 +25012,11 @@
       <c r="W29">
         <v>0.159805</v>
       </c>
+      <c r="X29">
+        <v>3.2516000000000003E-2</v>
+      </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>64</v>
       </c>
@@ -24247,6 +25029,9 @@
       <c r="E30">
         <v>0.17200599999999999</v>
       </c>
+      <c r="F30" s="3">
+        <v>0.12899099999999999</v>
+      </c>
       <c r="S30">
         <v>64</v>
       </c>
@@ -24259,8 +25044,11 @@
       <c r="W30">
         <v>0.16744700000000001</v>
       </c>
+      <c r="X30">
+        <v>2.6624999999999999E-2</v>
+      </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>128</v>
       </c>
@@ -24273,6 +25061,9 @@
       <c r="E31">
         <v>0.38206499999999999</v>
       </c>
+      <c r="F31" s="3">
+        <v>0.28734300000000002</v>
+      </c>
       <c r="S31">
         <v>128</v>
       </c>
@@ -24285,8 +25076,11 @@
       <c r="W31">
         <v>0.37980599999999998</v>
       </c>
+      <c r="X31">
+        <v>6.7829E-2</v>
+      </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>256</v>
       </c>
@@ -24299,6 +25093,9 @@
       <c r="E32">
         <v>0.87575800000000004</v>
       </c>
+      <c r="F32" s="3">
+        <v>0.443963</v>
+      </c>
       <c r="S32">
         <v>256</v>
       </c>
@@ -24311,20 +25108,23 @@
       <c r="W32">
         <v>0.85675699999999999</v>
       </c>
+      <c r="X32">
+        <v>0.153311</v>
+      </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="S34" s="3" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="S34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
+      <c r="T34" s="4"/>
+      <c r="U34" s="4"/>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -24362,7 +25162,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>8</v>
       </c>
@@ -24375,6 +25175,9 @@
       <c r="E36">
         <v>1.7006E-2</v>
       </c>
+      <c r="F36" s="3">
+        <v>6.2950000000000002E-3</v>
+      </c>
       <c r="S36">
         <v>8</v>
       </c>
@@ -24387,8 +25190,11 @@
       <c r="W36">
         <v>1.6605999999999999E-2</v>
       </c>
+      <c r="X36">
+        <v>1.5932000000000002E-2</v>
+      </c>
     </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>16</v>
       </c>
@@ -24401,6 +25207,9 @@
       <c r="E37">
         <v>2.5479999999999999E-2</v>
       </c>
+      <c r="F37" s="3">
+        <v>1.9459000000000001E-2</v>
+      </c>
       <c r="S37">
         <v>16</v>
       </c>
@@ -24413,8 +25222,11 @@
       <c r="W37">
         <v>2.4756E-2</v>
       </c>
+      <c r="X37">
+        <v>1.7932E-2</v>
+      </c>
     </row>
-    <row r="38" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>32</v>
       </c>
@@ -24427,6 +25239,9 @@
       <c r="E38">
         <v>1.6084000000000001E-2</v>
       </c>
+      <c r="F38" s="3">
+        <v>3.3668999999999998E-2</v>
+      </c>
       <c r="S38">
         <v>32</v>
       </c>
@@ -24439,8 +25254,11 @@
       <c r="W38">
         <v>1.4955E-2</v>
       </c>
+      <c r="X38">
+        <v>2.605E-2</v>
+      </c>
     </row>
-    <row r="39" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>64</v>
       </c>
@@ -24453,6 +25271,9 @@
       <c r="E39">
         <v>3.4081E-2</v>
       </c>
+      <c r="F39" s="3">
+        <v>2.0011999999999999E-2</v>
+      </c>
       <c r="S39">
         <v>64</v>
       </c>
@@ -24465,8 +25286,11 @@
       <c r="W39">
         <v>3.3153000000000002E-2</v>
       </c>
+      <c r="X39">
+        <v>3.2580999999999999E-2</v>
+      </c>
     </row>
-    <row r="40" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>128</v>
       </c>
@@ -24479,6 +25303,9 @@
       <c r="E40">
         <v>6.7832000000000003E-2</v>
       </c>
+      <c r="F40" s="3">
+        <v>5.7289E-2</v>
+      </c>
       <c r="S40">
         <v>128</v>
       </c>
@@ -24491,8 +25318,11 @@
       <c r="W40">
         <v>5.9919E-2</v>
       </c>
+      <c r="X40">
+        <v>6.3001000000000001E-2</v>
+      </c>
     </row>
-    <row r="41" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>256</v>
       </c>
@@ -24505,6 +25335,9 @@
       <c r="E41">
         <v>0.105521</v>
       </c>
+      <c r="F41" s="3">
+        <v>6.3159000000000007E-2</v>
+      </c>
       <c r="S41">
         <v>256</v>
       </c>
@@ -24517,8 +25350,11 @@
       <c r="W41">
         <v>9.6848000000000004E-2</v>
       </c>
+      <c r="X41">
+        <v>8.9913000000000007E-2</v>
+      </c>
     </row>
-    <row r="43" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -24556,7 +25392,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>8</v>
       </c>
@@ -24569,6 +25405,9 @@
       <c r="E44">
         <v>9.4900000000000002E-3</v>
       </c>
+      <c r="F44" s="3">
+        <v>1.1473000000000001E-2</v>
+      </c>
       <c r="S44">
         <v>8</v>
       </c>
@@ -24581,8 +25420,11 @@
       <c r="W44">
         <v>8.6859999999999993E-3</v>
       </c>
+      <c r="X44">
+        <v>1.8329999999999999E-2</v>
+      </c>
     </row>
-    <row r="45" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>16</v>
       </c>
@@ -24595,6 +25437,9 @@
       <c r="E45">
         <v>2.6797999999999999E-2</v>
       </c>
+      <c r="F45" s="3">
+        <v>2.8052000000000001E-2</v>
+      </c>
       <c r="S45">
         <v>16</v>
       </c>
@@ -24607,8 +25452,11 @@
       <c r="W45">
         <v>2.6269000000000001E-2</v>
       </c>
+      <c r="X45">
+        <v>1.4019E-2</v>
+      </c>
     </row>
-    <row r="46" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>32</v>
       </c>
@@ -24621,6 +25469,9 @@
       <c r="E46">
         <v>3.2382000000000001E-2</v>
       </c>
+      <c r="F46" s="3">
+        <v>2.2391999999999999E-2</v>
+      </c>
       <c r="S46">
         <v>32</v>
       </c>
@@ -24633,8 +25484,11 @@
       <c r="W46">
         <v>3.0828000000000001E-2</v>
       </c>
+      <c r="X46">
+        <v>2.3931000000000001E-2</v>
+      </c>
     </row>
-    <row r="47" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>64</v>
       </c>
@@ -24647,6 +25501,9 @@
       <c r="E47">
         <v>1.7281999999999999E-2</v>
       </c>
+      <c r="F47" s="3">
+        <v>6.2779999999999997E-3</v>
+      </c>
       <c r="S47">
         <v>64</v>
       </c>
@@ -24659,8 +25516,11 @@
       <c r="W47">
         <v>1.6936E-2</v>
       </c>
+      <c r="X47">
+        <v>2.5627E-2</v>
+      </c>
     </row>
-    <row r="48" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>128</v>
       </c>
@@ -24673,6 +25533,9 @@
       <c r="E48">
         <v>7.1410000000000001E-2</v>
       </c>
+      <c r="F48" s="3">
+        <v>5.3997999999999997E-2</v>
+      </c>
       <c r="S48">
         <v>128</v>
       </c>
@@ -24685,8 +25548,11 @@
       <c r="W48">
         <v>6.5180000000000002E-2</v>
       </c>
+      <c r="X48">
+        <v>8.4365999999999997E-2</v>
+      </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>256</v>
       </c>
@@ -24699,6 +25565,9 @@
       <c r="E49">
         <v>0.23064699999999999</v>
       </c>
+      <c r="F49" s="3">
+        <v>6.3769000000000006E-2</v>
+      </c>
       <c r="S49">
         <v>256</v>
       </c>
@@ -24711,8 +25580,11 @@
       <c r="W49">
         <v>0.23055899999999999</v>
       </c>
+      <c r="X49">
+        <v>3.5460999999999999E-2</v>
+      </c>
     </row>
-    <row r="51" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -24750,7 +25622,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>8</v>
       </c>
@@ -24763,6 +25635,9 @@
       <c r="E52">
         <v>3.9953000000000002E-2</v>
       </c>
+      <c r="F52" s="3">
+        <v>3.4338E-2</v>
+      </c>
       <c r="S52">
         <v>8</v>
       </c>
@@ -24775,8 +25650,11 @@
       <c r="W52">
         <v>3.8799E-2</v>
       </c>
+      <c r="X52">
+        <v>1.4937000000000001E-2</v>
+      </c>
     </row>
-    <row r="53" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>16</v>
       </c>
@@ -24789,6 +25667,9 @@
       <c r="E53">
         <v>2.5596000000000001E-2</v>
       </c>
+      <c r="F53" s="3">
+        <v>1.7707000000000001E-2</v>
+      </c>
       <c r="S53">
         <v>16</v>
       </c>
@@ -24801,8 +25682,11 @@
       <c r="W53">
         <v>2.4545999999999998E-2</v>
       </c>
+      <c r="X53">
+        <v>2.3643999999999998E-2</v>
+      </c>
     </row>
-    <row r="54" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>32</v>
       </c>
@@ -24815,6 +25699,9 @@
       <c r="E54">
         <v>2.8975999999999998E-2</v>
       </c>
+      <c r="F54" s="3">
+        <v>4.0133000000000002E-2</v>
+      </c>
       <c r="S54">
         <v>32</v>
       </c>
@@ -24827,8 +25714,11 @@
       <c r="W54">
         <v>2.801E-2</v>
       </c>
+      <c r="X54">
+        <v>3.8670000000000003E-2</v>
+      </c>
     </row>
-    <row r="55" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>64</v>
       </c>
@@ -24841,6 +25731,9 @@
       <c r="E55">
         <v>2.5992999999999999E-2</v>
       </c>
+      <c r="F55" s="3">
+        <v>3.3820999999999997E-2</v>
+      </c>
       <c r="S55">
         <v>64</v>
       </c>
@@ -24853,8 +25746,11 @@
       <c r="W55">
         <v>2.5808999999999999E-2</v>
       </c>
+      <c r="X55">
+        <v>2.9288999999999999E-2</v>
+      </c>
     </row>
-    <row r="56" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>128</v>
       </c>
@@ -24867,6 +25763,9 @@
       <c r="E56">
         <v>6.7111000000000004E-2</v>
       </c>
+      <c r="F56" s="3">
+        <v>4.8272000000000002E-2</v>
+      </c>
       <c r="S56">
         <v>128</v>
       </c>
@@ -24879,8 +25778,11 @@
       <c r="W56">
         <v>6.6985000000000003E-2</v>
       </c>
+      <c r="X56">
+        <v>0.10155500000000001</v>
+      </c>
     </row>
-    <row r="57" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>256</v>
       </c>
@@ -24893,6 +25795,9 @@
       <c r="E57">
         <v>0.16659599999999999</v>
       </c>
+      <c r="F57" s="3">
+        <v>8.2777000000000003E-2</v>
+      </c>
       <c r="S57">
         <v>256</v>
       </c>
@@ -24905,8 +25810,11 @@
       <c r="W57">
         <v>0.152951</v>
       </c>
+      <c r="X57">
+        <v>8.1212000000000006E-2</v>
+      </c>
     </row>
-    <row r="59" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -24944,7 +25852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="60" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>8</v>
       </c>
@@ -24957,6 +25865,9 @@
       <c r="E60">
         <v>9.1209999999999999E-2</v>
       </c>
+      <c r="F60" s="3">
+        <v>1.9216E-2</v>
+      </c>
       <c r="S60">
         <v>8</v>
       </c>
@@ -24969,8 +25880,11 @@
       <c r="W60">
         <v>8.1754999999999994E-2</v>
       </c>
+      <c r="X60">
+        <v>1.7901E-2</v>
+      </c>
     </row>
-    <row r="61" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>16</v>
       </c>
@@ -24983,6 +25897,9 @@
       <c r="E61">
         <v>9.0212000000000001E-2</v>
       </c>
+      <c r="F61" s="3">
+        <v>2.4427999999999998E-2</v>
+      </c>
       <c r="S61">
         <v>16</v>
       </c>
@@ -24995,8 +25912,11 @@
       <c r="W61">
         <v>8.4830000000000003E-2</v>
       </c>
+      <c r="X61">
+        <v>3.3878999999999999E-2</v>
+      </c>
     </row>
-    <row r="62" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>32</v>
       </c>
@@ -25009,6 +25929,9 @@
       <c r="E62">
         <v>0.110887</v>
       </c>
+      <c r="F62" s="3">
+        <v>4.0640000000000003E-2</v>
+      </c>
       <c r="S62">
         <v>32</v>
       </c>
@@ -25021,8 +25944,11 @@
       <c r="W62">
         <v>0.10824499999999999</v>
       </c>
+      <c r="X62">
+        <v>4.6337000000000003E-2</v>
+      </c>
     </row>
-    <row r="63" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>64</v>
       </c>
@@ -25035,6 +25961,9 @@
       <c r="E63">
         <v>9.8781999999999995E-2</v>
       </c>
+      <c r="F63" s="3">
+        <v>4.6342000000000001E-2</v>
+      </c>
       <c r="S63">
         <v>64</v>
       </c>
@@ -25047,8 +25976,11 @@
       <c r="W63">
         <v>9.7577999999999998E-2</v>
       </c>
+      <c r="X63">
+        <v>3.32E-2</v>
+      </c>
     </row>
-    <row r="64" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>128</v>
       </c>
@@ -25061,6 +25993,9 @@
       <c r="E64">
         <v>0.198708</v>
       </c>
+      <c r="F64" s="3">
+        <v>7.4229000000000003E-2</v>
+      </c>
       <c r="S64">
         <v>128</v>
       </c>
@@ -25073,8 +26008,11 @@
       <c r="W64">
         <v>0.19812199999999999</v>
       </c>
+      <c r="X64">
+        <v>8.4585999999999995E-2</v>
+      </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>256</v>
       </c>
@@ -25087,6 +26025,9 @@
       <c r="E65">
         <v>0.56554700000000002</v>
       </c>
+      <c r="F65" s="3">
+        <v>0.104893</v>
+      </c>
       <c r="S65">
         <v>256</v>
       </c>
@@ -25099,20 +26040,23 @@
       <c r="W65">
         <v>0.55332700000000001</v>
       </c>
+      <c r="X65">
+        <v>0.16179099999999999</v>
+      </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="S67" s="3" t="s">
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="S67" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -25150,7 +26094,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>8</v>
       </c>
@@ -25163,6 +26107,9 @@
       <c r="E69">
         <v>1.7080000000000001E-2</v>
       </c>
+      <c r="F69" s="3">
+        <v>8.5719999999999998E-3</v>
+      </c>
       <c r="S69">
         <v>8</v>
       </c>
@@ -25175,8 +26122,11 @@
       <c r="W69">
         <v>1.6695999999999999E-2</v>
       </c>
+      <c r="X69">
+        <v>1.8436999999999999E-2</v>
+      </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>16</v>
       </c>
@@ -25189,6 +26139,9 @@
       <c r="E70">
         <v>1.1963E-2</v>
       </c>
+      <c r="F70" s="3">
+        <v>2.0250000000000001E-2</v>
+      </c>
       <c r="S70">
         <v>16</v>
       </c>
@@ -25201,8 +26154,11 @@
       <c r="W70">
         <v>1.1194000000000001E-2</v>
       </c>
+      <c r="X70">
+        <v>1.2390999999999999E-2</v>
+      </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>32</v>
       </c>
@@ -25215,6 +26171,9 @@
       <c r="E71">
         <v>4.9942E-2</v>
       </c>
+      <c r="F71" s="3">
+        <v>3.1577000000000001E-2</v>
+      </c>
       <c r="S71">
         <v>32</v>
       </c>
@@ -25227,8 +26186,11 @@
       <c r="W71">
         <v>4.9525E-2</v>
       </c>
+      <c r="X71">
+        <v>2.3266999999999999E-2</v>
+      </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>64</v>
       </c>
@@ -25241,6 +26203,9 @@
       <c r="E72">
         <v>1.5923E-2</v>
       </c>
+      <c r="F72" s="3">
+        <v>2.2010999999999999E-2</v>
+      </c>
       <c r="S72">
         <v>64</v>
       </c>
@@ -25253,8 +26218,11 @@
       <c r="W72">
         <v>1.5346E-2</v>
       </c>
+      <c r="X72">
+        <v>1.2478E-2</v>
+      </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>128</v>
       </c>
@@ -25267,6 +26235,9 @@
       <c r="E73">
         <v>5.3751E-2</v>
       </c>
+      <c r="F73" s="3">
+        <v>2.1776E-2</v>
+      </c>
       <c r="S73">
         <v>128</v>
       </c>
@@ -25279,8 +26250,11 @@
       <c r="W73">
         <v>4.2127999999999999E-2</v>
       </c>
+      <c r="X73">
+        <v>3.1126999999999998E-2</v>
+      </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>256</v>
       </c>
@@ -25293,6 +26267,9 @@
       <c r="E74">
         <v>0.17565700000000001</v>
       </c>
+      <c r="F74" s="3">
+        <v>7.8702999999999995E-2</v>
+      </c>
       <c r="S74">
         <v>256</v>
       </c>
@@ -25305,8 +26282,11 @@
       <c r="W74">
         <v>0.169073</v>
       </c>
+      <c r="X74">
+        <v>8.1311999999999995E-2</v>
+      </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -25344,7 +26324,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>8</v>
       </c>
@@ -25357,6 +26337,9 @@
       <c r="E77">
         <v>8.4910000000000003E-3</v>
       </c>
+      <c r="F77" s="3">
+        <v>1.6642000000000001E-2</v>
+      </c>
       <c r="S77">
         <v>8</v>
       </c>
@@ -25369,8 +26352,11 @@
       <c r="W77">
         <v>7.5779999999999997E-3</v>
       </c>
+      <c r="X77">
+        <v>2.2051999999999999E-2</v>
+      </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>16</v>
       </c>
@@ -25383,6 +26369,9 @@
       <c r="E78">
         <v>1.9172000000000002E-2</v>
       </c>
+      <c r="F78" s="3">
+        <v>1.8213E-2</v>
+      </c>
       <c r="S78">
         <v>16</v>
       </c>
@@ -25395,8 +26384,11 @@
       <c r="W78">
         <v>1.8615E-2</v>
       </c>
+      <c r="X78">
+        <v>1.2297000000000001E-2</v>
+      </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>32</v>
       </c>
@@ -25409,6 +26401,9 @@
       <c r="E79">
         <v>4.0755E-2</v>
       </c>
+      <c r="F79" s="3">
+        <v>3.7397E-2</v>
+      </c>
       <c r="S79">
         <v>32</v>
       </c>
@@ -25421,8 +26416,11 @@
       <c r="W79">
         <v>4.0323999999999999E-2</v>
       </c>
+      <c r="X79">
+        <v>5.0191E-2</v>
+      </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>64</v>
       </c>
@@ -25435,6 +26433,9 @@
       <c r="E80">
         <v>9.7890000000000008E-3</v>
       </c>
+      <c r="F80" s="3">
+        <v>3.2160000000000001E-3</v>
+      </c>
       <c r="S80">
         <v>64</v>
       </c>
@@ -25447,8 +26448,11 @@
       <c r="W80">
         <v>9.214E-3</v>
       </c>
+      <c r="X80">
+        <v>1.9289000000000001E-2</v>
+      </c>
     </row>
-    <row r="81" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>128</v>
       </c>
@@ -25461,6 +26465,9 @@
       <c r="E81">
         <v>6.1765E-2</v>
       </c>
+      <c r="F81" s="3">
+        <v>4.5702E-2</v>
+      </c>
       <c r="S81">
         <v>128</v>
       </c>
@@ -25473,8 +26480,11 @@
       <c r="W81">
         <v>5.9046000000000001E-2</v>
       </c>
+      <c r="X81">
+        <v>7.3955999999999994E-2</v>
+      </c>
     </row>
-    <row r="82" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>256</v>
       </c>
@@ -25487,6 +26497,9 @@
       <c r="E82">
         <v>0.16472999999999999</v>
       </c>
+      <c r="F82" s="3">
+        <v>6.0645999999999999E-2</v>
+      </c>
       <c r="S82">
         <v>256</v>
       </c>
@@ -25499,8 +26512,11 @@
       <c r="W82">
         <v>0.13297500000000001</v>
       </c>
+      <c r="X82">
+        <v>0.13647699999999999</v>
+      </c>
     </row>
-    <row r="84" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -25538,7 +26554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="85" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>8</v>
       </c>
@@ -25551,6 +26567,9 @@
       <c r="E85">
         <v>2.7614E-2</v>
       </c>
+      <c r="F85" s="3">
+        <v>1.3943000000000001E-2</v>
+      </c>
       <c r="S85">
         <v>8</v>
       </c>
@@ -25563,8 +26582,11 @@
       <c r="W85">
         <v>2.5940000000000001E-2</v>
       </c>
+      <c r="X85">
+        <v>1.4508999999999999E-2</v>
+      </c>
     </row>
-    <row r="86" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>16</v>
       </c>
@@ -25577,6 +26599,9 @@
       <c r="E86">
         <v>2.9433999999999998E-2</v>
       </c>
+      <c r="F86" s="3">
+        <v>1.8565999999999999E-2</v>
+      </c>
       <c r="S86">
         <v>16</v>
       </c>
@@ -25589,8 +26614,11 @@
       <c r="W86">
         <v>2.8344999999999999E-2</v>
       </c>
+      <c r="X86">
+        <v>1.6212000000000001E-2</v>
+      </c>
     </row>
-    <row r="87" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>32</v>
       </c>
@@ -25603,6 +26631,9 @@
       <c r="E87">
         <v>4.6836000000000003E-2</v>
       </c>
+      <c r="F87" s="3">
+        <v>2.8176E-2</v>
+      </c>
       <c r="S87">
         <v>32</v>
       </c>
@@ -25615,8 +26646,11 @@
       <c r="W87">
         <v>4.5185000000000003E-2</v>
       </c>
+      <c r="X87">
+        <v>3.2460999999999997E-2</v>
+      </c>
     </row>
-    <row r="88" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>64</v>
       </c>
@@ -25629,6 +26663,9 @@
       <c r="E88">
         <v>3.4745999999999999E-2</v>
       </c>
+      <c r="F88" s="3">
+        <v>2.2918000000000001E-2</v>
+      </c>
       <c r="S88">
         <v>64</v>
       </c>
@@ -25641,8 +26678,11 @@
       <c r="W88">
         <v>3.4556000000000003E-2</v>
       </c>
+      <c r="X88">
+        <v>1.524E-2</v>
+      </c>
     </row>
-    <row r="89" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>128</v>
       </c>
@@ -25655,6 +26695,9 @@
       <c r="E89">
         <v>6.5581E-2</v>
       </c>
+      <c r="F89" s="3">
+        <v>4.4602000000000003E-2</v>
+      </c>
       <c r="S89">
         <v>128</v>
       </c>
@@ -25667,8 +26710,11 @@
       <c r="W89">
         <v>6.0690000000000001E-2</v>
       </c>
+      <c r="X89">
+        <v>8.3803000000000002E-2</v>
+      </c>
     </row>
-    <row r="90" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>256</v>
       </c>
@@ -25681,6 +26727,9 @@
       <c r="E90">
         <v>0.16339799999999999</v>
       </c>
+      <c r="F90" s="3">
+        <v>9.8957000000000003E-2</v>
+      </c>
       <c r="S90">
         <v>256</v>
       </c>
@@ -25693,8 +26742,11 @@
       <c r="W90">
         <v>0.160995</v>
       </c>
+      <c r="X90">
+        <v>0.15889</v>
+      </c>
     </row>
-    <row r="92" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -25732,7 +26784,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="93" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>8</v>
       </c>
@@ -25745,6 +26797,9 @@
       <c r="E93">
         <v>9.9562999999999999E-2</v>
       </c>
+      <c r="F93" s="3">
+        <v>2.104E-2</v>
+      </c>
       <c r="S93">
         <v>8</v>
       </c>
@@ -25757,8 +26812,11 @@
       <c r="W93">
         <v>8.9981000000000005E-2</v>
       </c>
+      <c r="X93">
+        <v>2.1561E-2</v>
+      </c>
     </row>
-    <row r="94" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>16</v>
       </c>
@@ -25771,6 +26829,9 @@
       <c r="E94">
         <v>9.2874999999999999E-2</v>
       </c>
+      <c r="F94" s="3">
+        <v>2.6762000000000001E-2</v>
+      </c>
       <c r="S94">
         <v>16</v>
       </c>
@@ -25783,8 +26844,11 @@
       <c r="W94">
         <v>8.8151999999999994E-2</v>
       </c>
+      <c r="X94">
+        <v>3.8799E-2</v>
+      </c>
     </row>
-    <row r="95" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>32</v>
       </c>
@@ -25797,6 +26861,9 @@
       <c r="E95">
         <v>0.109123</v>
       </c>
+      <c r="F95" s="3">
+        <v>3.6427000000000001E-2</v>
+      </c>
       <c r="S95">
         <v>32</v>
       </c>
@@ -25809,8 +26876,11 @@
       <c r="W95">
         <v>9.1856999999999994E-2</v>
       </c>
+      <c r="X95">
+        <v>4.0637E-2</v>
+      </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>64</v>
       </c>
@@ -25823,6 +26893,9 @@
       <c r="E96">
         <v>0.16328699999999999</v>
       </c>
+      <c r="F96" s="3">
+        <v>3.6237999999999999E-2</v>
+      </c>
       <c r="S96">
         <v>64</v>
       </c>
@@ -25835,8 +26908,11 @@
       <c r="W96">
         <v>0.16197600000000001</v>
       </c>
+      <c r="X96">
+        <v>4.2352000000000001E-2</v>
+      </c>
     </row>
-    <row r="97" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>128</v>
       </c>
@@ -25849,6 +26925,9 @@
       <c r="E97">
         <v>0.183536</v>
       </c>
+      <c r="F97" s="3">
+        <v>7.1371000000000004E-2</v>
+      </c>
       <c r="S97">
         <v>128</v>
       </c>
@@ -25861,8 +26940,11 @@
       <c r="W97">
         <v>0.170323</v>
       </c>
+      <c r="X97">
+        <v>8.5550000000000001E-2</v>
+      </c>
     </row>
-    <row r="98" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>256</v>
       </c>
@@ -25875,6 +26957,9 @@
       <c r="E98">
         <v>0.46755000000000002</v>
       </c>
+      <c r="F98" s="3">
+        <v>0.101713</v>
+      </c>
       <c r="S98">
         <v>256</v>
       </c>
@@ -25887,20 +26972,23 @@
       <c r="W98">
         <v>0.46067200000000003</v>
       </c>
+      <c r="X98">
+        <v>0.157607</v>
+      </c>
     </row>
-    <row r="100" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
+    <row r="100" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="S100" s="3" t="s">
+      <c r="B100" s="4"/>
+      <c r="C100" s="4"/>
+      <c r="S100" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="T100" s="3"/>
-      <c r="U100" s="3"/>
+      <c r="T100" s="4"/>
+      <c r="U100" s="4"/>
     </row>
-    <row r="101" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -25929,7 +27017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="102" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>8</v>
       </c>
@@ -25951,8 +27039,11 @@
       <c r="W102">
         <v>3.6999999999999998E-5</v>
       </c>
+      <c r="X102">
+        <v>8.175E-3</v>
+      </c>
     </row>
-    <row r="103" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>16</v>
       </c>
@@ -25974,8 +27065,11 @@
       <c r="W103">
         <v>2.6999999999999999E-5</v>
       </c>
+      <c r="X103">
+        <v>8.9789999999999991E-3</v>
+      </c>
     </row>
-    <row r="104" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>32</v>
       </c>
@@ -25997,8 +27091,11 @@
       <c r="W104">
         <v>1.8E-5</v>
       </c>
+      <c r="X104">
+        <v>1.6871000000000001E-2</v>
+      </c>
     </row>
-    <row r="105" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>64</v>
       </c>
@@ -26020,8 +27117,11 @@
       <c r="W105">
         <v>1.5E-5</v>
       </c>
+      <c r="X105">
+        <v>2.1998E-2</v>
+      </c>
     </row>
-    <row r="106" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>128</v>
       </c>
@@ -26043,8 +27143,11 @@
       <c r="W106">
         <v>6.9999999999999999E-6</v>
       </c>
+      <c r="X106">
+        <v>5.1069999999999997E-2</v>
+      </c>
     </row>
-    <row r="107" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>256</v>
       </c>
@@ -26066,8 +27169,11 @@
       <c r="W107">
         <v>7.9999999999999996E-6</v>
       </c>
+      <c r="X107">
+        <v>0.135628</v>
+      </c>
     </row>
-    <row r="109" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -26096,7 +27202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="110" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>8</v>
       </c>
@@ -26118,8 +27224,11 @@
       <c r="W110">
         <v>2.7399999999999999E-4</v>
       </c>
+      <c r="X110">
+        <v>6.4549999999999998E-3</v>
+      </c>
     </row>
-    <row r="111" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>16</v>
       </c>
@@ -26141,8 +27250,11 @@
       <c r="W111">
         <v>1.36E-4</v>
       </c>
+      <c r="X111">
+        <v>1.9907000000000001E-2</v>
+      </c>
     </row>
-    <row r="112" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>32</v>
       </c>
@@ -26164,8 +27276,11 @@
       <c r="W112">
         <v>8.2000000000000001E-5</v>
       </c>
+      <c r="X112">
+        <v>2.1572999999999998E-2</v>
+      </c>
     </row>
-    <row r="113" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>64</v>
       </c>
@@ -26187,8 +27302,11 @@
       <c r="W113">
         <v>4.6999999999999997E-5</v>
       </c>
+      <c r="X113">
+        <v>2.2851E-2</v>
+      </c>
     </row>
-    <row r="114" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>128</v>
       </c>
@@ -26210,8 +27328,11 @@
       <c r="W114">
         <v>3.6999999999999998E-5</v>
       </c>
+      <c r="X114">
+        <v>7.2641999999999998E-2</v>
+      </c>
     </row>
-    <row r="115" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>256</v>
       </c>
@@ -26233,8 +27354,11 @@
       <c r="W115">
         <v>1.12E-4</v>
       </c>
+      <c r="X115">
+        <v>0.116288</v>
+      </c>
     </row>
-    <row r="117" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>0</v>
       </c>
@@ -26263,7 +27387,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="118" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>8</v>
       </c>
@@ -26285,8 +27409,11 @@
       <c r="W118">
         <v>3.3909999999999999E-3</v>
       </c>
+      <c r="X118">
+        <v>1.0068000000000001E-2</v>
+      </c>
     </row>
-    <row r="119" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>16</v>
       </c>
@@ -26308,8 +27435,11 @@
       <c r="W119">
         <v>1.555E-3</v>
       </c>
+      <c r="X119">
+        <v>8.7519999999999994E-3</v>
+      </c>
     </row>
-    <row r="120" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>32</v>
       </c>
@@ -26331,8 +27461,11 @@
       <c r="W120">
         <v>7.1299999999999998E-4</v>
       </c>
+      <c r="X120">
+        <v>1.3837E-2</v>
+      </c>
     </row>
-    <row r="121" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>64</v>
       </c>
@@ -26354,8 +27487,11 @@
       <c r="W121">
         <v>3.6099999999999999E-4</v>
       </c>
+      <c r="X121">
+        <v>1.6997999999999999E-2</v>
+      </c>
     </row>
-    <row r="122" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>128</v>
       </c>
@@ -26377,8 +27513,11 @@
       <c r="W122">
         <v>1.8699999999999999E-4</v>
       </c>
+      <c r="X122">
+        <v>6.5725000000000006E-2</v>
+      </c>
     </row>
-    <row r="123" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>256</v>
       </c>
@@ -26400,8 +27539,11 @@
       <c r="W123">
         <v>8.7000000000000001E-5</v>
       </c>
+      <c r="X123">
+        <v>0.165934</v>
+      </c>
     </row>
-    <row r="125" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>0</v>
       </c>
@@ -26430,7 +27572,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="126" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>8</v>
       </c>
@@ -26452,8 +27594,11 @@
       <c r="W126">
         <v>3.6357E-2</v>
       </c>
+      <c r="X126">
+        <v>1.4394000000000001E-2</v>
+      </c>
     </row>
-    <row r="127" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>16</v>
       </c>
@@ -26475,8 +27620,11 @@
       <c r="W127">
         <v>1.7686E-2</v>
       </c>
+      <c r="X127">
+        <v>8.1939999999999999E-3</v>
+      </c>
     </row>
-    <row r="128" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>32</v>
       </c>
@@ -26498,8 +27646,11 @@
       <c r="W128">
         <v>8.7899999999999992E-3</v>
       </c>
+      <c r="X128">
+        <v>1.9265000000000001E-2</v>
+      </c>
     </row>
-    <row r="129" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>64</v>
       </c>
@@ -26521,8 +27672,11 @@
       <c r="W129">
         <v>3.9379999999999997E-3</v>
       </c>
+      <c r="X129">
+        <v>1.3268E-2</v>
+      </c>
     </row>
-    <row r="130" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>128</v>
       </c>
@@ -26544,8 +27698,11 @@
       <c r="W130">
         <v>2.215E-3</v>
       </c>
+      <c r="X130">
+        <v>6.7829E-2</v>
+      </c>
     </row>
-    <row r="131" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>256</v>
       </c>
@@ -26567,15 +27724,18 @@
       <c r="W131">
         <v>1.3749999999999999E-3</v>
       </c>
+      <c r="X131">
+        <v>0.145428</v>
+      </c>
     </row>
-    <row r="133" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="S133" s="3" t="s">
+    <row r="133" spans="1:24" x14ac:dyDescent="0.3">
+      <c r="S133" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="T133" s="3"/>
-      <c r="U133" s="3"/>
+      <c r="T133" s="4"/>
+      <c r="U133" s="4"/>
     </row>
-    <row r="134" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S134" t="s">
         <v>0</v>
       </c>
@@ -26595,7 +27755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="135" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S135">
         <v>8</v>
       </c>
@@ -26608,8 +27768,11 @@
       <c r="W135">
         <v>2.0999999999999999E-5</v>
       </c>
+      <c r="X135">
+        <v>7.7590000000000003E-3</v>
+      </c>
     </row>
-    <row r="136" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S136">
         <v>16</v>
       </c>
@@ -26622,8 +27785,11 @@
       <c r="W136">
         <v>2.6999999999999999E-5</v>
       </c>
+      <c r="X136">
+        <v>7.5329999999999998E-3</v>
+      </c>
     </row>
-    <row r="137" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S137">
         <v>32</v>
       </c>
@@ -26636,8 +27802,11 @@
       <c r="W137">
         <v>2.5000000000000001E-5</v>
       </c>
+      <c r="X137">
+        <v>1.0697999999999999E-2</v>
+      </c>
     </row>
-    <row r="138" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S138">
         <v>64</v>
       </c>
@@ -26650,8 +27819,11 @@
       <c r="W138">
         <v>1.8E-5</v>
       </c>
+      <c r="X138">
+        <v>1.5703999999999999E-2</v>
+      </c>
     </row>
-    <row r="139" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S139">
         <v>128</v>
       </c>
@@ -26664,8 +27836,11 @@
       <c r="W139">
         <v>8.5000000000000006E-5</v>
       </c>
+      <c r="X139">
+        <v>6.2245000000000002E-2</v>
+      </c>
     </row>
-    <row r="140" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S140">
         <v>256</v>
       </c>
@@ -26678,8 +27853,11 @@
       <c r="W140">
         <v>6.0000000000000002E-6</v>
       </c>
+      <c r="X140">
+        <v>0.103587</v>
+      </c>
     </row>
-    <row r="142" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S142" t="s">
         <v>0</v>
       </c>
@@ -26699,7 +27877,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="143" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S143">
         <v>8</v>
       </c>
@@ -26712,8 +27890,11 @@
       <c r="W143">
         <v>8.2999999999999998E-5</v>
       </c>
+      <c r="X143">
+        <v>8.8669999999999999E-3</v>
+      </c>
     </row>
-    <row r="144" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:24" x14ac:dyDescent="0.3">
       <c r="S144">
         <v>16</v>
       </c>
@@ -26726,8 +27907,11 @@
       <c r="W144">
         <v>5.0000000000000002E-5</v>
       </c>
+      <c r="X144">
+        <v>6.293E-3</v>
+      </c>
     </row>
-    <row r="145" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="145" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S145">
         <v>32</v>
       </c>
@@ -26740,8 +27924,11 @@
       <c r="W145">
         <v>3.0000000000000001E-5</v>
       </c>
+      <c r="X145">
+        <v>9.0530000000000003E-3</v>
+      </c>
     </row>
-    <row r="146" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="146" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S146">
         <v>64</v>
       </c>
@@ -26754,8 +27941,11 @@
       <c r="W146">
         <v>2.5999999999999998E-5</v>
       </c>
+      <c r="X146">
+        <v>1.4133E-2</v>
+      </c>
     </row>
-    <row r="147" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="147" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S147">
         <v>128</v>
       </c>
@@ -26768,8 +27958,11 @@
       <c r="W147">
         <v>1.8E-5</v>
       </c>
+      <c r="X147">
+        <v>7.1854000000000001E-2</v>
+      </c>
     </row>
-    <row r="148" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="148" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S148">
         <v>256</v>
       </c>
@@ -26782,8 +27975,11 @@
       <c r="W148">
         <v>5.3999999999999998E-5</v>
       </c>
+      <c r="X148">
+        <v>0.108679</v>
+      </c>
     </row>
-    <row r="150" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="150" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S150" t="s">
         <v>0</v>
       </c>
@@ -26803,7 +27999,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="151" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="151" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S151">
         <v>8</v>
       </c>
@@ -26816,8 +28012,11 @@
       <c r="W151">
         <v>7.0799999999999997E-4</v>
       </c>
+      <c r="X151">
+        <v>7.5989999999999999E-3</v>
+      </c>
     </row>
-    <row r="152" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="152" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S152">
         <v>16</v>
       </c>
@@ -26830,8 +28029,11 @@
       <c r="W152">
         <v>3.8699999999999997E-4</v>
       </c>
+      <c r="X152">
+        <v>6.6519999999999999E-3</v>
+      </c>
     </row>
-    <row r="153" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="153" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S153">
         <v>32</v>
       </c>
@@ -26844,8 +28046,11 @@
       <c r="W153">
         <v>1.92E-4</v>
       </c>
+      <c r="X153">
+        <v>2.0392E-2</v>
+      </c>
     </row>
-    <row r="154" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="154" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S154">
         <v>64</v>
       </c>
@@ -26858,8 +28063,11 @@
       <c r="W154">
         <v>1.08E-4</v>
       </c>
+      <c r="X154">
+        <v>2.0022999999999999E-2</v>
+      </c>
     </row>
-    <row r="155" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="155" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S155">
         <v>128</v>
       </c>
@@ -26872,8 +28080,11 @@
       <c r="W155">
         <v>5.3000000000000001E-5</v>
       </c>
+      <c r="X155">
+        <v>7.1121000000000004E-2</v>
+      </c>
     </row>
-    <row r="156" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="156" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S156">
         <v>256</v>
       </c>
@@ -26886,8 +28097,11 @@
       <c r="W156">
         <v>3.4E-5</v>
       </c>
+      <c r="X156">
+        <v>0.11643199999999999</v>
+      </c>
     </row>
-    <row r="158" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="158" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S158" t="s">
         <v>0</v>
       </c>
@@ -26907,7 +28121,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="159" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="159" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S159">
         <v>8</v>
       </c>
@@ -26920,8 +28134,11 @@
       <c r="W159">
         <v>8.3829999999999998E-3</v>
       </c>
+      <c r="X159">
+        <v>8.2959999999999996E-3</v>
+      </c>
     </row>
-    <row r="160" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="160" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S160">
         <v>16</v>
       </c>
@@ -26934,8 +28151,11 @@
       <c r="W160">
         <v>3.823E-3</v>
       </c>
+      <c r="X160">
+        <v>1.9436999999999999E-2</v>
+      </c>
     </row>
-    <row r="161" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="161" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S161">
         <v>32</v>
       </c>
@@ -26948,8 +28168,11 @@
       <c r="W161">
         <v>1.853E-3</v>
       </c>
+      <c r="X161">
+        <v>2.1850000000000001E-2</v>
+      </c>
     </row>
-    <row r="162" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="162" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S162">
         <v>64</v>
       </c>
@@ -26962,8 +28185,11 @@
       <c r="W162">
         <v>9.0799999999999995E-4</v>
       </c>
+      <c r="X162">
+        <v>3.4317E-2</v>
+      </c>
     </row>
-    <row r="163" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="163" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S163">
         <v>128</v>
       </c>
@@ -26976,8 +28202,11 @@
       <c r="W163">
         <v>6.1600000000000001E-4</v>
       </c>
+      <c r="X163">
+        <v>8.2733000000000001E-2</v>
+      </c>
     </row>
-    <row r="164" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="164" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S164">
         <v>256</v>
       </c>
@@ -26990,15 +28219,18 @@
       <c r="W164">
         <v>2.4899999999999998E-4</v>
       </c>
+      <c r="X164">
+        <v>0.16811899999999999</v>
+      </c>
     </row>
-    <row r="166" spans="19:24" x14ac:dyDescent="0.25">
-      <c r="S166" s="3" t="s">
+    <row r="166" spans="19:24" x14ac:dyDescent="0.3">
+      <c r="S166" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="T166" s="3"/>
-      <c r="U166" s="3"/>
+      <c r="T166" s="4"/>
+      <c r="U166" s="4"/>
     </row>
-    <row r="167" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="167" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S167" t="s">
         <v>0</v>
       </c>
@@ -27018,7 +28250,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="168" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="168" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S168">
         <v>8</v>
       </c>
@@ -27031,8 +28263,11 @@
       <c r="W168">
         <v>2.4000000000000001E-5</v>
       </c>
+      <c r="X168">
+        <v>1.1310000000000001E-2</v>
+      </c>
     </row>
-    <row r="169" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="169" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S169">
         <v>16</v>
       </c>
@@ -27045,8 +28280,11 @@
       <c r="W169">
         <v>2.5000000000000001E-5</v>
       </c>
+      <c r="X169">
+        <v>4.0429999999999997E-3</v>
+      </c>
     </row>
-    <row r="170" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="170" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S170">
         <v>32</v>
       </c>
@@ -27059,8 +28297,11 @@
       <c r="W170">
         <v>1.5999999999999999E-5</v>
       </c>
+      <c r="X170">
+        <v>8.7390000000000002E-3</v>
+      </c>
     </row>
-    <row r="171" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="171" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S171">
         <v>64</v>
       </c>
@@ -27073,8 +28314,11 @@
       <c r="W171">
         <v>1.4E-5</v>
       </c>
+      <c r="X171">
+        <v>1.6081999999999999E-2</v>
+      </c>
     </row>
-    <row r="172" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="172" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S172">
         <v>128</v>
       </c>
@@ -27087,8 +28331,11 @@
       <c r="W172">
         <v>6.4999999999999994E-5</v>
       </c>
+      <c r="X172">
+        <v>5.2253000000000001E-2</v>
+      </c>
     </row>
-    <row r="173" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="173" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S173">
         <v>256</v>
       </c>
@@ -27101,8 +28348,11 @@
       <c r="W173">
         <v>6.0000000000000002E-6</v>
       </c>
+      <c r="X173">
+        <v>9.1018000000000002E-2</v>
+      </c>
     </row>
-    <row r="175" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="175" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S175" t="s">
         <v>0</v>
       </c>
@@ -27122,7 +28372,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="176" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="176" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S176">
         <v>8</v>
       </c>
@@ -27135,8 +28385,11 @@
       <c r="W176">
         <v>7.7999999999999999E-5</v>
       </c>
+      <c r="X176">
+        <v>1.1221E-2</v>
+      </c>
     </row>
-    <row r="177" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="177" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S177">
         <v>16</v>
       </c>
@@ -27149,8 +28402,11 @@
       <c r="W177">
         <v>4.6E-5</v>
       </c>
+      <c r="X177">
+        <v>6.2329999999999998E-3</v>
+      </c>
     </row>
-    <row r="178" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="178" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S178">
         <v>32</v>
       </c>
@@ -27163,8 +28419,11 @@
       <c r="W178">
         <v>3.8000000000000002E-5</v>
       </c>
+      <c r="X178">
+        <v>2.545E-2</v>
+      </c>
     </row>
-    <row r="179" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="179" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S179">
         <v>64</v>
       </c>
@@ -27177,8 +28436,11 @@
       <c r="W179">
         <v>2.9E-5</v>
       </c>
+      <c r="X179">
+        <v>2.5004999999999999E-2</v>
+      </c>
     </row>
-    <row r="180" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="180" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S180">
         <v>128</v>
       </c>
@@ -27191,8 +28453,11 @@
       <c r="W180">
         <v>1.8E-5</v>
       </c>
+      <c r="X180">
+        <v>6.4911999999999997E-2</v>
+      </c>
     </row>
-    <row r="181" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="181" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S181">
         <v>256</v>
       </c>
@@ -27205,8 +28470,11 @@
       <c r="W181">
         <v>1.5999999999999999E-5</v>
       </c>
+      <c r="X181">
+        <v>0.121527</v>
+      </c>
     </row>
-    <row r="183" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="183" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S183" t="s">
         <v>0</v>
       </c>
@@ -27226,7 +28494,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="184" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="184" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S184">
         <v>8</v>
       </c>
@@ -27239,8 +28507,11 @@
       <c r="W184">
         <v>7.3499999999999998E-4</v>
       </c>
+      <c r="X184">
+        <v>8.3099999999999997E-3</v>
+      </c>
     </row>
-    <row r="185" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="185" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S185">
         <v>16</v>
       </c>
@@ -27253,8 +28524,11 @@
       <c r="W185">
         <v>3.8299999999999999E-4</v>
       </c>
+      <c r="X185">
+        <v>9.7040000000000008E-3</v>
+      </c>
     </row>
-    <row r="186" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="186" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S186">
         <v>32</v>
       </c>
@@ -27267,8 +28541,11 @@
       <c r="W186">
         <v>2.0000000000000001E-4</v>
       </c>
+      <c r="X186">
+        <v>1.8169999999999999E-2</v>
+      </c>
     </row>
-    <row r="187" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="187" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S187">
         <v>64</v>
       </c>
@@ -27281,8 +28558,11 @@
       <c r="W187">
         <v>1.1E-4</v>
       </c>
+      <c r="X187">
+        <v>1.8797999999999999E-2</v>
+      </c>
     </row>
-    <row r="188" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="188" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S188">
         <v>128</v>
       </c>
@@ -27295,8 +28575,11 @@
       <c r="W188">
         <v>5.3999999999999998E-5</v>
       </c>
+      <c r="X188">
+        <v>8.3127000000000006E-2</v>
+      </c>
     </row>
-    <row r="189" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="189" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S189">
         <v>256</v>
       </c>
@@ -27309,8 +28592,11 @@
       <c r="W189">
         <v>3.4999999999999997E-5</v>
       </c>
+      <c r="X189">
+        <v>0.153255</v>
+      </c>
     </row>
-    <row r="191" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="191" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S191" t="s">
         <v>0</v>
       </c>
@@ -27330,7 +28616,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="192" spans="19:24" x14ac:dyDescent="0.25">
+    <row r="192" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S192">
         <v>8</v>
       </c>
@@ -27343,8 +28629,11 @@
       <c r="W192">
         <v>8.2019999999999992E-3</v>
       </c>
+      <c r="X192">
+        <v>1.2034E-2</v>
+      </c>
     </row>
-    <row r="193" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="193" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S193">
         <v>16</v>
       </c>
@@ -27357,8 +28646,11 @@
       <c r="W193">
         <v>4.0340000000000003E-3</v>
       </c>
+      <c r="X193">
+        <v>3.0501E-2</v>
+      </c>
     </row>
-    <row r="194" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="194" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S194">
         <v>32</v>
       </c>
@@ -27371,8 +28663,11 @@
       <c r="W194">
         <v>2.1510000000000001E-3</v>
       </c>
+      <c r="X194">
+        <v>2.7268000000000001E-2</v>
+      </c>
     </row>
-    <row r="195" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="195" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S195">
         <v>64</v>
       </c>
@@ -27385,8 +28680,11 @@
       <c r="W195">
         <v>1.3209999999999999E-3</v>
       </c>
+      <c r="X195">
+        <v>3.4879E-2</v>
+      </c>
     </row>
-    <row r="196" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="196" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S196">
         <v>128</v>
       </c>
@@ -27399,8 +28697,11 @@
       <c r="W196">
         <v>6.0700000000000001E-4</v>
       </c>
+      <c r="X196">
+        <v>8.5350999999999996E-2</v>
+      </c>
     </row>
-    <row r="197" spans="19:23" x14ac:dyDescent="0.25">
+    <row r="197" spans="19:24" x14ac:dyDescent="0.3">
       <c r="S197">
         <v>256</v>
       </c>
@@ -27412,6 +28713,9 @@
       </c>
       <c r="W197">
         <v>4.1800000000000002E-4</v>
+      </c>
+      <c r="X197">
+        <v>0.17979700000000001</v>
       </c>
     </row>
   </sheetData>
@@ -27441,21 +28745,21 @@
       <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.109375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -27471,7 +28775,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>19</v>
       </c>
@@ -27485,7 +28789,7 @@
         <v>22.587736</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C3">
         <v>400</v>
       </c>
@@ -27493,7 +28797,7 @@
         <v>68.031053</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C4">
         <v>600</v>
       </c>
@@ -27501,7 +28805,7 @@
         <v>96.859639000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C5">
         <v>800</v>
       </c>
@@ -27509,7 +28813,7 @@
         <v>133.09767600000001</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C6">
         <v>1000</v>
       </c>
@@ -27517,7 +28821,7 @@
         <v>105.33103300000001</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>17</v>
       </c>
@@ -27528,7 +28832,7 @@
         <v>22.132449999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C8">
         <v>400</v>
       </c>
@@ -27536,7 +28840,7 @@
         <v>68.324811999999994</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C9">
         <v>600</v>
       </c>
@@ -27544,7 +28848,7 @@
         <v>99.867918000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C10">
         <v>800</v>
       </c>
@@ -27552,7 +28856,7 @@
         <v>144.118911</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C11">
         <v>1000</v>
       </c>
@@ -27560,7 +28864,7 @@
         <v>107.818224</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>18</v>
       </c>
@@ -27571,7 +28875,7 @@
         <v>22.143097000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C13">
         <v>400</v>
       </c>
@@ -27579,7 +28883,7 @@
         <v>68.969154000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C14">
         <v>600</v>
       </c>
@@ -27587,7 +28891,7 @@
         <v>99.088296999999997</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C15">
         <v>800</v>
       </c>
@@ -27595,7 +28899,7 @@
         <v>135.47776200000001</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C16">
         <v>1000</v>
       </c>
@@ -27603,7 +28907,7 @@
         <v>108.44539399999999</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -27617,7 +28921,7 @@
         <v>20.385031000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C18">
         <v>400</v>
       </c>
@@ -27625,7 +28929,7 @@
         <v>62.713659999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C19">
         <v>600</v>
       </c>
@@ -27633,7 +28937,7 @@
         <v>87.318619999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C20">
         <v>800</v>
       </c>
@@ -27641,7 +28945,7 @@
         <v>124.902693</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C21">
         <v>1000</v>
       </c>
@@ -27649,7 +28953,7 @@
         <v>105.117226</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>17</v>
       </c>
@@ -27660,7 +28964,7 @@
         <v>20.857983000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C23">
         <v>400</v>
       </c>
@@ -27668,7 +28972,7 @@
         <v>62.655282999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C24">
         <v>600</v>
       </c>
@@ -27676,7 +28980,7 @@
         <v>88.825207000000006</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C25">
         <v>800</v>
       </c>
@@ -27684,7 +28988,7 @@
         <v>132.33948699999999</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C26">
         <v>1000</v>
       </c>
@@ -27692,7 +28996,7 @@
         <v>105.238286</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>18</v>
       </c>
@@ -27703,7 +29007,7 @@
         <v>20.026244999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C28">
         <v>400</v>
       </c>
@@ -27711,7 +29015,7 @@
         <v>63.102696999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C29">
         <v>600</v>
       </c>
@@ -27719,7 +29023,7 @@
         <v>89.439897999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C30">
         <v>800</v>
       </c>
@@ -27727,7 +29031,7 @@
         <v>133.184684</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C31">
         <v>1000</v>
       </c>
@@ -27735,7 +29039,7 @@
         <v>105.223328</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -27749,7 +29053,7 @@
         <v>21.345030999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C33">
         <v>400</v>
       </c>
@@ -27757,7 +29061,7 @@
         <v>60.753160000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C34">
         <v>600</v>
       </c>
@@ -27767,7 +29071,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C35">
         <v>800</v>
       </c>
@@ -27775,7 +29079,7 @@
         <v>122.909273</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C36">
         <v>1000</v>
       </c>
@@ -27783,7 +29087,7 @@
         <v>104.324226</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>17</v>
       </c>
@@ -27794,7 +29098,7 @@
         <v>19.287382999999998</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C38">
         <v>400</v>
       </c>
@@ -27802,7 +29106,7 @@
         <v>61.918375300000001</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C39">
         <v>600</v>
       </c>
@@ -27810,7 +29114,7 @@
         <v>90.825207000000006</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C40">
         <v>800</v>
       </c>
@@ -27818,7 +29122,7 @@
         <v>134.382487</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C41">
         <v>1000</v>
       </c>
@@ -27826,7 +29130,7 @@
         <v>104.928471</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>18</v>
       </c>
@@ -27837,7 +29141,7 @@
         <v>21.026292999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C43">
         <v>400</v>
       </c>
@@ -27845,7 +29149,7 @@
         <v>65.191697000000005</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C44">
         <v>600</v>
       </c>
@@ -27853,7 +29157,7 @@
         <v>88.439193000000003</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C45">
         <v>800</v>
       </c>
@@ -27861,7 +29165,7 @@
         <v>133.18284199999999</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C46">
         <v>1000</v>
       </c>
@@ -27869,7 +29173,7 @@
         <v>106.119483</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -27880,7 +29184,7 @@
         <v>8.8839999999999995E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C48">
         <v>400</v>
       </c>
@@ -27888,7 +29192,7 @@
         <v>1.694E-2</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C49">
         <v>600</v>
       </c>
@@ -27896,7 +29200,7 @@
         <v>2.7026999999999999E-2</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C50">
         <v>800</v>
       </c>
@@ -27904,7 +29208,7 @@
         <v>3.0908000000000001E-2</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C51">
         <v>1000</v>
       </c>
@@ -27912,27 +29216,27 @@
         <v>3.3589000000000001E-2</v>
       </c>
     </row>
-    <row r="67" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" s="2"/>
       <c r="B92" s="2"/>
     </row>
-    <row r="100" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S100" s="1"/>
       <c r="T100" s="1"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A125" s="2"/>
       <c r="B125" s="2"/>
     </row>
-    <row r="133" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S133" s="1"/>
       <c r="T133" s="1"/>
     </row>
-    <row r="166" spans="19:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="19:20" x14ac:dyDescent="0.3">
       <c r="S166" s="1"/>
       <c r="T166" s="1"/>
     </row>

</xml_diff>